<commit_message>
update to parsed modules spreadsheet
</commit_message>
<xml_diff>
--- a/parsed_modules.xlsx
+++ b/parsed_modules.xlsx
@@ -1,24 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/ucapcjg_ucl_ac_uk/Documents/Work/GitHubRepos/hpc-spack/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:40009_{763C7209-7DDC-4B1B-B313-E43AE37FF459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{974FF99A-F3CB-4BC7-8A9E-89C9D7947FAA}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:40009_{763C7209-7DDC-4B1B-B313-E43AE37FF459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37A89742-ABBC-4F85-9783-2EF395E8BA13}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="912" yWindow="912" windowWidth="23304" windowHeight="13224" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{ABCE3EB6-57D9-41B5-BABF-9E2F88F42FD5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parsed_modules" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5432" uniqueCount="1571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5437" uniqueCount="1573">
   <si>
     <t>package</t>
   </si>
@@ -4749,6 +4747,12 @@
   </si>
   <si>
     <t>sys     372m17.225s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">package made </t>
+  </si>
+  <si>
+    <t>1.11.1.1208</t>
   </si>
 </sst>
 </file>
@@ -5346,10 +5350,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5647,33 +5647,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q463"/>
+  <dimension ref="A1:R463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A291" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A281" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="Q298" sqref="Q298"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.21875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.21875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.21875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="29.21875" style="1" customWidth="1"/>
-    <col min="9" max="10" width="15.44140625" customWidth="1"/>
-    <col min="11" max="11" width="22.44140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="29.28515625" style="1" customWidth="1"/>
+    <col min="9" max="10" width="15.42578125" customWidth="1"/>
+    <col min="11" max="11" width="49.5703125" customWidth="1"/>
     <col min="12" max="12" width="17" customWidth="1"/>
-    <col min="13" max="13" width="6.21875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="16.77734375" customWidth="1"/>
-    <col min="15" max="15" width="22.21875" customWidth="1"/>
+    <col min="13" max="13" width="6.28515625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" customWidth="1"/>
+    <col min="15" max="15" width="22.28515625" customWidth="1"/>
+    <col min="16" max="16" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5714,7 +5714,7 @@
         <v>1494</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>43</v>
       </c>
@@ -5749,7 +5749,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
@@ -5787,7 +5787,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>53</v>
       </c>
@@ -5825,7 +5825,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>56</v>
       </c>
@@ -5860,7 +5860,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>59</v>
       </c>
@@ -5898,7 +5898,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>64</v>
       </c>
@@ -5933,7 +5933,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>67</v>
       </c>
@@ -5971,7 +5971,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>70</v>
       </c>
@@ -6006,7 +6006,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>73</v>
       </c>
@@ -6044,7 +6044,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>76</v>
       </c>
@@ -6079,7 +6079,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>79</v>
       </c>
@@ -6114,7 +6114,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>82</v>
       </c>
@@ -6152,7 +6152,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>85</v>
       </c>
@@ -6190,7 +6190,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>88</v>
       </c>
@@ -6225,7 +6225,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>91</v>
       </c>
@@ -6263,7 +6263,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>94</v>
       </c>
@@ -6298,7 +6298,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>97</v>
       </c>
@@ -6333,7 +6333,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>100</v>
       </c>
@@ -6368,7 +6368,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>103</v>
       </c>
@@ -6403,7 +6403,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>106</v>
       </c>
@@ -6438,7 +6438,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>109</v>
       </c>
@@ -6473,7 +6473,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>112</v>
       </c>
@@ -6508,7 +6508,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>116</v>
       </c>
@@ -6546,7 +6546,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>119</v>
       </c>
@@ -6584,7 +6584,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>122</v>
       </c>
@@ -6622,7 +6622,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>125</v>
       </c>
@@ -6660,7 +6660,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>136</v>
       </c>
@@ -6695,7 +6695,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>140</v>
       </c>
@@ -6733,7 +6733,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>143</v>
       </c>
@@ -6771,7 +6771,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>147</v>
       </c>
@@ -6806,7 +6806,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>150</v>
       </c>
@@ -6841,7 +6841,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>154</v>
       </c>
@@ -6876,7 +6876,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>157</v>
       </c>
@@ -6911,7 +6911,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>162</v>
       </c>
@@ -6949,7 +6949,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>165</v>
       </c>
@@ -6984,7 +6984,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>168</v>
       </c>
@@ -7019,7 +7019,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>171</v>
       </c>
@@ -7054,7 +7054,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>174</v>
       </c>
@@ -7089,7 +7089,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>177</v>
       </c>
@@ -7124,7 +7124,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>180</v>
       </c>
@@ -7159,7 +7159,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>183</v>
       </c>
@@ -7194,7 +7194,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>187</v>
       </c>
@@ -7232,7 +7232,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>193</v>
       </c>
@@ -7270,7 +7270,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>197</v>
       </c>
@@ -7305,7 +7305,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>200</v>
       </c>
@@ -7340,7 +7340,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>202</v>
       </c>
@@ -7378,7 +7378,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>205</v>
       </c>
@@ -7416,7 +7416,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>208</v>
       </c>
@@ -7454,7 +7454,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>211</v>
       </c>
@@ -7492,7 +7492,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>216</v>
       </c>
@@ -7530,7 +7530,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>219</v>
       </c>
@@ -7565,7 +7565,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>222</v>
       </c>
@@ -7600,7 +7600,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>226</v>
       </c>
@@ -7638,7 +7638,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>230</v>
       </c>
@@ -7673,7 +7673,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>233</v>
       </c>
@@ -7708,7 +7708,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>239</v>
       </c>
@@ -7746,7 +7746,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>246</v>
       </c>
@@ -7784,7 +7784,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>249</v>
       </c>
@@ -7822,7 +7822,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>252</v>
       </c>
@@ -7857,7 +7857,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>258</v>
       </c>
@@ -7892,7 +7892,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>255</v>
       </c>
@@ -7930,7 +7930,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>261</v>
       </c>
@@ -7965,7 +7965,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>264</v>
       </c>
@@ -8003,7 +8003,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>268</v>
       </c>
@@ -8041,7 +8041,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>272</v>
       </c>
@@ -8076,7 +8076,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>275</v>
       </c>
@@ -8111,7 +8111,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>278</v>
       </c>
@@ -8149,7 +8149,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>281</v>
       </c>
@@ -8187,7 +8187,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>284</v>
       </c>
@@ -8225,7 +8225,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>287</v>
       </c>
@@ -8263,7 +8263,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>290</v>
       </c>
@@ -8301,7 +8301,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>292</v>
       </c>
@@ -8336,7 +8336,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>295</v>
       </c>
@@ -8374,7 +8374,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>298</v>
       </c>
@@ -8409,7 +8409,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>301</v>
       </c>
@@ -8447,7 +8447,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>304</v>
       </c>
@@ -8485,7 +8485,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>309</v>
       </c>
@@ -8520,7 +8520,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>312</v>
       </c>
@@ -8558,7 +8558,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>315</v>
       </c>
@@ -8596,7 +8596,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>319</v>
       </c>
@@ -8634,7 +8634,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>322</v>
       </c>
@@ -8672,7 +8672,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>325</v>
       </c>
@@ -8707,7 +8707,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>328</v>
       </c>
@@ -8745,7 +8745,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>331</v>
       </c>
@@ -8783,7 +8783,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>338</v>
       </c>
@@ -8821,7 +8821,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>341</v>
       </c>
@@ -8859,7 +8859,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>344</v>
       </c>
@@ -8897,7 +8897,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="89" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>347</v>
       </c>
@@ -8935,7 +8935,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>350</v>
       </c>
@@ -8973,7 +8973,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>353</v>
       </c>
@@ -9011,7 +9011,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>362</v>
       </c>
@@ -9049,7 +9049,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>365</v>
       </c>
@@ -9087,7 +9087,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>368</v>
       </c>
@@ -9122,7 +9122,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>371</v>
       </c>
@@ -9157,7 +9157,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>374</v>
       </c>
@@ -9195,7 +9195,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>377</v>
       </c>
@@ -9230,7 +9230,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>380</v>
       </c>
@@ -9268,7 +9268,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>383</v>
       </c>
@@ -9303,7 +9303,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>387</v>
       </c>
@@ -9338,7 +9338,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>390</v>
       </c>
@@ -9376,7 +9376,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="102" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>393</v>
       </c>
@@ -9411,7 +9411,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>396</v>
       </c>
@@ -9449,7 +9449,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="104" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>399</v>
       </c>
@@ -9484,7 +9484,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>402</v>
       </c>
@@ -9522,7 +9522,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="106" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>405</v>
       </c>
@@ -9557,7 +9557,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>408</v>
       </c>
@@ -9595,7 +9595,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="108" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>414</v>
       </c>
@@ -9633,7 +9633,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>418</v>
       </c>
@@ -9671,7 +9671,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="110" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>421</v>
       </c>
@@ -9706,7 +9706,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>424</v>
       </c>
@@ -9741,7 +9741,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>427</v>
       </c>
@@ -9776,7 +9776,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="113" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>430</v>
       </c>
@@ -9814,7 +9814,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="114" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>437</v>
       </c>
@@ -9852,7 +9852,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="115" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>440</v>
       </c>
@@ -9890,7 +9890,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="116" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>443</v>
       </c>
@@ -9928,7 +9928,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="117" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>447</v>
       </c>
@@ -9966,7 +9966,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="118" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>450</v>
       </c>
@@ -10004,7 +10004,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>454</v>
       </c>
@@ -10042,7 +10042,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>457</v>
       </c>
@@ -10077,7 +10077,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="121" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>460</v>
       </c>
@@ -10112,7 +10112,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="122" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>463</v>
       </c>
@@ -10150,7 +10150,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="123" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>466</v>
       </c>
@@ -10185,7 +10185,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="124" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>470</v>
       </c>
@@ -10220,7 +10220,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="125" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>473</v>
       </c>
@@ -10258,7 +10258,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="126" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>477</v>
       </c>
@@ -10293,7 +10293,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="127" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>482</v>
       </c>
@@ -10331,7 +10331,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="128" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>486</v>
       </c>
@@ -10366,7 +10366,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="129" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>490</v>
       </c>
@@ -10401,7 +10401,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="130" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>493</v>
       </c>
@@ -10439,7 +10439,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="131" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>497</v>
       </c>
@@ -10477,7 +10477,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="132" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>500</v>
       </c>
@@ -10515,7 +10515,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="133" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>503</v>
       </c>
@@ -10550,7 +10550,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="134" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>506</v>
       </c>
@@ -10588,7 +10588,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="135" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>512</v>
       </c>
@@ -10626,7 +10626,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="136" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>515</v>
       </c>
@@ -10664,7 +10664,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="137" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>522</v>
       </c>
@@ -10699,7 +10699,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="138" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>525</v>
       </c>
@@ -10734,7 +10734,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="139" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>528</v>
       </c>
@@ -10769,7 +10769,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="140" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>531</v>
       </c>
@@ -10804,7 +10804,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="141" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>534</v>
       </c>
@@ -10842,7 +10842,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="142" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>539</v>
       </c>
@@ -10877,7 +10877,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="143" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>546</v>
       </c>
@@ -10915,7 +10915,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="144" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>550</v>
       </c>
@@ -10953,7 +10953,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="145" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>553</v>
       </c>
@@ -10991,7 +10991,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="146" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>556</v>
       </c>
@@ -11029,7 +11029,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="147" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>560</v>
       </c>
@@ -11064,7 +11064,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>564</v>
       </c>
@@ -11102,7 +11102,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="149" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>568</v>
       </c>
@@ -11140,7 +11140,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="150" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>571</v>
       </c>
@@ -11175,7 +11175,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="151" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>574</v>
       </c>
@@ -11213,7 +11213,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="152" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>578</v>
       </c>
@@ -11251,7 +11251,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="153" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>581</v>
       </c>
@@ -11289,7 +11289,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="154" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>584</v>
       </c>
@@ -11327,7 +11327,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="155" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>587</v>
       </c>
@@ -11365,7 +11365,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="156" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>590</v>
       </c>
@@ -11400,7 +11400,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="157" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>593</v>
       </c>
@@ -11438,7 +11438,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="158" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>596</v>
       </c>
@@ -11473,7 +11473,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="159" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>599</v>
       </c>
@@ -11508,7 +11508,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="160" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>602</v>
       </c>
@@ -11546,7 +11546,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="161" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>605</v>
       </c>
@@ -11584,7 +11584,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="162" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>610</v>
       </c>
@@ -11622,7 +11622,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="163" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>614</v>
       </c>
@@ -11660,7 +11660,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="164" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>618</v>
       </c>
@@ -11695,7 +11695,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="165" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>621</v>
       </c>
@@ -11733,7 +11733,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="166" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>624</v>
       </c>
@@ -11771,7 +11771,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="167" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>627</v>
       </c>
@@ -11806,7 +11806,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="168" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>630</v>
       </c>
@@ -11841,7 +11841,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="169" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>633</v>
       </c>
@@ -11876,7 +11876,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="170" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>636</v>
       </c>
@@ -11911,7 +11911,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="171" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>639</v>
       </c>
@@ -11946,7 +11946,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="172" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>642</v>
       </c>
@@ -11981,7 +11981,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="173" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>645</v>
       </c>
@@ -12016,7 +12016,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="174" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>648</v>
       </c>
@@ -12054,7 +12054,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="175" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>659</v>
       </c>
@@ -12092,7 +12092,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="176" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>662</v>
       </c>
@@ -12130,7 +12130,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="177" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>665</v>
       </c>
@@ -12165,7 +12165,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="178" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>667</v>
       </c>
@@ -12203,7 +12203,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="179" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>672</v>
       </c>
@@ -12238,7 +12238,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="180" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>677</v>
       </c>
@@ -12276,7 +12276,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="181" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>680</v>
       </c>
@@ -12311,7 +12311,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="182" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>682</v>
       </c>
@@ -12346,7 +12346,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="183" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>685</v>
       </c>
@@ -12384,7 +12384,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="184" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>688</v>
       </c>
@@ -12422,7 +12422,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="185" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>692</v>
       </c>
@@ -12460,7 +12460,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="186" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>695</v>
       </c>
@@ -12495,7 +12495,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="187" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>699</v>
       </c>
@@ -12533,7 +12533,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="188" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>702</v>
       </c>
@@ -12568,7 +12568,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="189" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>705</v>
       </c>
@@ -12603,7 +12603,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="190" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>708</v>
       </c>
@@ -12641,7 +12641,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="191" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>711</v>
       </c>
@@ -12676,7 +12676,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="192" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>714</v>
       </c>
@@ -12714,7 +12714,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="193" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>717</v>
       </c>
@@ -12749,7 +12749,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="194" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>721</v>
       </c>
@@ -12787,7 +12787,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="195" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>724</v>
       </c>
@@ -12822,7 +12822,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="196" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>727</v>
       </c>
@@ -12857,7 +12857,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="197" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>730</v>
       </c>
@@ -12895,7 +12895,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="198" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>734</v>
       </c>
@@ -12930,7 +12930,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="199" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>737</v>
       </c>
@@ -12968,7 +12968,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="200" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>740</v>
       </c>
@@ -13006,7 +13006,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="201" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>743</v>
       </c>
@@ -13044,7 +13044,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="202" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>746</v>
       </c>
@@ -13079,7 +13079,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="203" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>749</v>
       </c>
@@ -13114,7 +13114,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="204" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>752</v>
       </c>
@@ -13152,7 +13152,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="205" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>755</v>
       </c>
@@ -13187,7 +13187,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="206" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>758</v>
       </c>
@@ -13222,7 +13222,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="207" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>761</v>
       </c>
@@ -13257,7 +13257,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="208" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>767</v>
       </c>
@@ -13292,7 +13292,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="209" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>771</v>
       </c>
@@ -13330,7 +13330,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="210" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>774</v>
       </c>
@@ -13374,7 +13374,7 @@
         <v>1528</v>
       </c>
     </row>
-    <row r="211" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>777</v>
       </c>
@@ -13412,7 +13412,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="212" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>780</v>
       </c>
@@ -13447,7 +13447,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="213" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>783</v>
       </c>
@@ -13485,7 +13485,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="214" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>786</v>
       </c>
@@ -13523,7 +13523,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="215" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>788</v>
       </c>
@@ -13561,7 +13561,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="216" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>791</v>
       </c>
@@ -13596,7 +13596,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="217" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>793</v>
       </c>
@@ -13634,7 +13634,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="218" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>796</v>
       </c>
@@ -13669,7 +13669,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="219" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>799</v>
       </c>
@@ -13707,7 +13707,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="220" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>802</v>
       </c>
@@ -13745,7 +13745,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="221" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>806</v>
       </c>
@@ -13780,7 +13780,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="222" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>809</v>
       </c>
@@ -13818,7 +13818,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="223" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>812</v>
       </c>
@@ -13856,7 +13856,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="224" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>815</v>
       </c>
@@ -13894,7 +13894,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="225" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>821</v>
       </c>
@@ -13932,7 +13932,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="226" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>824</v>
       </c>
@@ -13970,7 +13970,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="227" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>827</v>
       </c>
@@ -14005,7 +14005,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="228" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>830</v>
       </c>
@@ -14043,7 +14043,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="229" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>834</v>
       </c>
@@ -14078,7 +14078,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="230" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>837</v>
       </c>
@@ -14116,7 +14116,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="231" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>840</v>
       </c>
@@ -14151,7 +14151,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="232" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>842</v>
       </c>
@@ -14189,7 +14189,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="233" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>845</v>
       </c>
@@ -14227,7 +14227,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="234" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>849</v>
       </c>
@@ -14265,7 +14265,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="235" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>852</v>
       </c>
@@ -14300,7 +14300,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="236" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>855</v>
       </c>
@@ -14335,7 +14335,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="237" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>858</v>
       </c>
@@ -14370,7 +14370,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="238" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>861</v>
       </c>
@@ -14408,7 +14408,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="239" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>1445</v>
       </c>
@@ -14443,7 +14443,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="240" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>1447</v>
       </c>
@@ -14478,7 +14478,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="241" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>1449</v>
       </c>
@@ -14513,7 +14513,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="242" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>1450</v>
       </c>
@@ -14548,7 +14548,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="243" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>129</v>
       </c>
@@ -14583,7 +14583,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="244" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>1452</v>
       </c>
@@ -14618,7 +14618,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="245" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>1454</v>
       </c>
@@ -14653,7 +14653,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="246" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>1456</v>
       </c>
@@ -14688,7 +14688,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="247" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>1458</v>
       </c>
@@ -14723,7 +14723,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="248" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>1461</v>
       </c>
@@ -14758,7 +14758,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="249" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>1463</v>
       </c>
@@ -14793,7 +14793,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="250" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>1465</v>
       </c>
@@ -14828,7 +14828,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="251" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>1467</v>
       </c>
@@ -14863,7 +14863,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="252" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>335</v>
       </c>
@@ -14901,7 +14901,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="253" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>1469</v>
       </c>
@@ -14936,7 +14936,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="254" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>1471</v>
       </c>
@@ -14971,7 +14971,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="255" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>543</v>
       </c>
@@ -15009,7 +15009,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="256" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>1476</v>
       </c>
@@ -15044,7 +15044,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="257" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>1478</v>
       </c>
@@ -15079,7 +15079,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="258" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>1378</v>
       </c>
@@ -15114,7 +15114,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="259" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>1480</v>
       </c>
@@ -15149,7 +15149,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="260" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>1482</v>
       </c>
@@ -15184,7 +15184,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="261" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>654</v>
       </c>
@@ -15222,7 +15222,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="262" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>1486</v>
       </c>
@@ -15257,7 +15257,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="263" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>1487</v>
       </c>
@@ -15292,7 +15292,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="264" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>1489</v>
       </c>
@@ -15327,7 +15327,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="265" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>1491</v>
       </c>
@@ -15362,7 +15362,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="266" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>1224</v>
       </c>
@@ -15397,7 +15397,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="267" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>1227</v>
       </c>
@@ -15432,7 +15432,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="268" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>1229</v>
       </c>
@@ -15470,7 +15470,7 @@
         <v>1229</v>
       </c>
     </row>
-    <row r="269" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>1081</v>
       </c>
@@ -15508,7 +15508,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="270" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>1105</v>
       </c>
@@ -15546,7 +15546,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="271" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>1232</v>
       </c>
@@ -15581,7 +15581,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="272" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>1236</v>
       </c>
@@ -15619,7 +15619,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="273" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
         <v>1241</v>
       </c>
@@ -15657,7 +15657,7 @@
         <v>1241</v>
       </c>
     </row>
-    <row r="274" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
         <v>11</v>
       </c>
@@ -15692,7 +15692,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="275" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
         <v>15</v>
       </c>
@@ -15727,7 +15727,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="276" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>18</v>
       </c>
@@ -15762,7 +15762,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="277" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
         <v>21</v>
       </c>
@@ -15797,7 +15797,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="278" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>24</v>
       </c>
@@ -15832,7 +15832,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="279" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
         <v>27</v>
       </c>
@@ -15870,7 +15870,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="280" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
         <v>30</v>
       </c>
@@ -15905,7 +15905,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="281" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
         <v>32</v>
       </c>
@@ -15943,7 +15943,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="282" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
         <v>35</v>
       </c>
@@ -15981,7 +15981,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="283" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
         <v>38</v>
       </c>
@@ -16016,7 +16016,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="284" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
         <v>40</v>
       </c>
@@ -16051,7 +16051,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="285" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
         <v>1244</v>
       </c>
@@ -16086,7 +16086,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="286" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
         <v>1248</v>
       </c>
@@ -16130,7 +16130,7 @@
         <v>2.69</v>
       </c>
     </row>
-    <row r="287" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
         <v>1251</v>
       </c>
@@ -16171,7 +16171,7 @@
         <v>1251</v>
       </c>
     </row>
-    <row r="288" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
         <v>1254</v>
       </c>
@@ -16218,7 +16218,7 @@
         <v>1524</v>
       </c>
     </row>
-    <row r="289" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>1257</v>
       </c>
@@ -16262,7 +16262,7 @@
         <v>1530</v>
       </c>
     </row>
-    <row r="290" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
         <v>1260</v>
       </c>
@@ -16303,7 +16303,7 @@
         <v>2.38</v>
       </c>
     </row>
-    <row r="291" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
         <v>1263</v>
       </c>
@@ -16344,7 +16344,7 @@
         <v>1531</v>
       </c>
     </row>
-    <row r="292" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>1266</v>
       </c>
@@ -16378,8 +16378,14 @@
       <c r="L292" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="293" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P292" t="s">
+        <v>1571</v>
+      </c>
+      <c r="Q292" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="293" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
         <v>1269</v>
       </c>
@@ -16413,8 +16419,17 @@
       <c r="L293" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="294" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P293" t="s">
+        <v>1571</v>
+      </c>
+      <c r="Q293" t="s">
+        <v>1269</v>
+      </c>
+      <c r="R293" t="s">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="294" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
         <v>1272</v>
       </c>
@@ -16455,7 +16470,7 @@
         <v>1532</v>
       </c>
     </row>
-    <row r="295" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
         <v>1275</v>
       </c>
@@ -16493,7 +16508,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="296" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
         <v>1278</v>
       </c>
@@ -16531,7 +16546,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="297" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
         <v>1281</v>
       </c>
@@ -16569,7 +16584,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="298" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
         <v>1285</v>
       </c>
@@ -16610,7 +16625,7 @@
         <v>1550</v>
       </c>
     </row>
-    <row r="299" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
         <v>1288</v>
       </c>
@@ -16645,7 +16660,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="300" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
         <v>1291</v>
       </c>
@@ -16683,7 +16698,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="301" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
         <v>1294</v>
       </c>
@@ -16721,7 +16736,7 @@
         <v>1294</v>
       </c>
     </row>
-    <row r="302" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
         <v>1297</v>
       </c>
@@ -16759,7 +16774,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="303" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
         <v>1300</v>
       </c>
@@ -16797,7 +16812,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="304" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
         <v>1303</v>
       </c>
@@ -16835,7 +16850,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="305" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
         <v>1306</v>
       </c>
@@ -16873,7 +16888,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="306" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
         <v>1309</v>
       </c>
@@ -16911,7 +16926,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="307" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
         <v>1312</v>
       </c>
@@ -16949,7 +16964,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="308" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
         <v>1314</v>
       </c>
@@ -16987,7 +17002,7 @@
         <v>1314</v>
       </c>
     </row>
-    <row r="309" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
         <v>1317</v>
       </c>
@@ -17022,7 +17037,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="310" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
         <v>1320</v>
       </c>
@@ -17060,7 +17075,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="311" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
         <v>1322</v>
       </c>
@@ -17095,7 +17110,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="312" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
         <v>1327</v>
       </c>
@@ -17133,7 +17148,7 @@
         <v>1327</v>
       </c>
     </row>
-    <row r="313" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
         <v>1330</v>
       </c>
@@ -17177,7 +17192,7 @@
         <v>1527</v>
       </c>
     </row>
-    <row r="314" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
         <v>1333</v>
       </c>
@@ -17215,7 +17230,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="315" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
         <v>1336</v>
       </c>
@@ -17253,7 +17268,7 @@
         <v>1336</v>
       </c>
     </row>
-    <row r="316" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
         <v>1339</v>
       </c>
@@ -17291,7 +17306,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="317" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
         <v>1342</v>
       </c>
@@ -17329,7 +17344,7 @@
         <v>1342</v>
       </c>
     </row>
-    <row r="318" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
         <v>1345</v>
       </c>
@@ -17367,7 +17382,7 @@
         <v>1345</v>
       </c>
     </row>
-    <row r="319" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
         <v>1348</v>
       </c>
@@ -17405,7 +17420,7 @@
         <v>1348</v>
       </c>
     </row>
-    <row r="320" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
         <v>1351</v>
       </c>
@@ -17443,7 +17458,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="321" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A321" s="1" t="s">
         <v>1354</v>
       </c>
@@ -17478,7 +17493,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="322" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
         <v>1357</v>
       </c>
@@ -17513,7 +17528,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="323" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
         <v>1360</v>
       </c>
@@ -17551,7 +17566,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="324" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
         <v>1363</v>
       </c>
@@ -17589,7 +17604,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="325" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
         <v>1366</v>
       </c>
@@ -17624,7 +17639,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="326" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
         <v>1369</v>
       </c>
@@ -17662,7 +17677,7 @@
         <v>1369</v>
       </c>
     </row>
-    <row r="327" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A327" s="1" t="s">
         <v>1372</v>
       </c>
@@ -17703,7 +17718,7 @@
         <v>1529</v>
       </c>
     </row>
-    <row r="328" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
         <v>1375</v>
       </c>
@@ -17738,7 +17753,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="329" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
         <v>1383</v>
       </c>
@@ -17776,7 +17791,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="330" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A330" s="1" t="s">
         <v>1388</v>
       </c>
@@ -17814,7 +17829,7 @@
         <v>1388</v>
       </c>
     </row>
-    <row r="331" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
         <v>1391</v>
       </c>
@@ -17852,7 +17867,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="332" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
         <v>1394</v>
       </c>
@@ -17890,7 +17905,7 @@
         <v>1394</v>
       </c>
     </row>
-    <row r="333" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
         <v>1397</v>
       </c>
@@ -17925,7 +17940,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="334" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
         <v>1400</v>
       </c>
@@ -17960,7 +17975,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="335" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
         <v>1403</v>
       </c>
@@ -17998,7 +18013,7 @@
         <v>1403</v>
       </c>
     </row>
-    <row r="336" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
         <v>1406</v>
       </c>
@@ -18033,7 +18048,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="337" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
         <v>1409</v>
       </c>
@@ -18068,7 +18083,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="338" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
         <v>1412</v>
       </c>
@@ -18106,7 +18121,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="339" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
         <v>1415</v>
       </c>
@@ -18144,7 +18159,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="340" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
         <v>1418</v>
       </c>
@@ -18182,7 +18197,7 @@
         <v>1418</v>
       </c>
     </row>
-    <row r="341" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
         <v>1421</v>
       </c>
@@ -18220,7 +18235,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="342" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
         <v>1424</v>
       </c>
@@ -18258,7 +18273,7 @@
         <v>1424</v>
       </c>
     </row>
-    <row r="343" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
         <v>1427</v>
       </c>
@@ -18296,7 +18311,7 @@
         <v>1427</v>
       </c>
     </row>
-    <row r="344" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
         <v>1430</v>
       </c>
@@ -18334,7 +18349,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="345" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="s">
         <v>1433</v>
       </c>
@@ -18369,7 +18384,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="346" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
         <v>1436</v>
       </c>
@@ -18407,7 +18422,7 @@
         <v>1436</v>
       </c>
     </row>
-    <row r="347" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
         <v>1439</v>
       </c>
@@ -18442,7 +18457,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="348" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
         <v>1442</v>
       </c>
@@ -18477,7 +18492,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="349" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
         <v>864</v>
       </c>
@@ -18515,7 +18530,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="350" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
         <v>867</v>
       </c>
@@ -18553,7 +18568,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="351" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A351" s="1" t="s">
         <v>870</v>
       </c>
@@ -18591,7 +18606,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="352" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A352" s="1" t="s">
         <v>873</v>
       </c>
@@ -18629,7 +18644,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="353" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A353" s="1" t="s">
         <v>876</v>
       </c>
@@ -18667,7 +18682,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="354" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
         <v>882</v>
       </c>
@@ -18705,7 +18720,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="355" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
         <v>885</v>
       </c>
@@ -18740,7 +18755,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="356" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
         <v>888</v>
       </c>
@@ -18778,7 +18793,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="357" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A357" s="1" t="s">
         <v>894</v>
       </c>
@@ -18813,7 +18828,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="358" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
         <v>897</v>
       </c>
@@ -18851,7 +18866,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="359" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A359" s="1" t="s">
         <v>900</v>
       </c>
@@ -18889,7 +18904,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="360" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
         <v>903</v>
       </c>
@@ -18924,7 +18939,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="361" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A361" s="1" t="s">
         <v>906</v>
       </c>
@@ -18962,7 +18977,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="362" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
         <v>909</v>
       </c>
@@ -19000,7 +19015,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="363" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A363" s="1" t="s">
         <v>912</v>
       </c>
@@ -19035,7 +19050,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="364" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
         <v>914</v>
       </c>
@@ -19073,7 +19088,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="365" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A365" s="1" t="s">
         <v>917</v>
       </c>
@@ -19111,7 +19126,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="366" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A366" s="1" t="s">
         <v>920</v>
       </c>
@@ -19149,7 +19164,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="367" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A367" s="1" t="s">
         <v>923</v>
       </c>
@@ -19187,7 +19202,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="368" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A368" s="1" t="s">
         <v>930</v>
       </c>
@@ -19222,7 +19237,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="369" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A369" s="1" t="s">
         <v>932</v>
       </c>
@@ -19260,7 +19275,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="370" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A370" s="1" t="s">
         <v>935</v>
       </c>
@@ -19298,7 +19313,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="371" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A371" s="1" t="s">
         <v>938</v>
       </c>
@@ -19333,7 +19348,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="372" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A372" s="1" t="s">
         <v>943</v>
       </c>
@@ -19368,7 +19383,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="373" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
         <v>946</v>
       </c>
@@ -19406,7 +19421,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="374" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
         <v>948</v>
       </c>
@@ -19444,7 +19459,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="375" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
         <v>950</v>
       </c>
@@ -19482,7 +19497,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="376" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
         <v>953</v>
       </c>
@@ -19517,7 +19532,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="377" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A377" s="1" t="s">
         <v>955</v>
       </c>
@@ -19555,7 +19570,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="378" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A378" s="1" t="s">
         <v>958</v>
       </c>
@@ -19593,7 +19608,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="379" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A379" s="1" t="s">
         <v>961</v>
       </c>
@@ -19631,7 +19646,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="380" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
         <v>964</v>
       </c>
@@ -19669,7 +19684,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="381" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A381" s="1" t="s">
         <v>967</v>
       </c>
@@ -19707,7 +19722,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="382" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A382" s="1" t="s">
         <v>970</v>
       </c>
@@ -19742,7 +19757,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="383" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A383" s="1" t="s">
         <v>357</v>
       </c>
@@ -19777,7 +19792,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="384" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A384" s="1" t="s">
         <v>973</v>
       </c>
@@ -19812,7 +19827,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="385" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A385" s="1" t="s">
         <v>977</v>
       </c>
@@ -19850,7 +19865,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="386" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A386" s="1" t="s">
         <v>980</v>
       </c>
@@ -19888,7 +19903,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="387" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A387" s="1" t="s">
         <v>986</v>
       </c>
@@ -19926,7 +19941,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="388" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A388" s="1" t="s">
         <v>989</v>
       </c>
@@ -19964,7 +19979,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="389" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A389" s="1" t="s">
         <v>992</v>
       </c>
@@ -20002,7 +20017,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="390" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A390" s="1" t="s">
         <v>996</v>
       </c>
@@ -20040,7 +20055,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="391" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A391" s="1" t="s">
         <v>999</v>
       </c>
@@ -20078,7 +20093,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="392" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A392" s="1" t="s">
         <v>1002</v>
       </c>
@@ -20116,7 +20131,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="393" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A393" s="1" t="s">
         <v>1005</v>
       </c>
@@ -20151,7 +20166,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="394" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A394" s="1" t="s">
         <v>1008</v>
       </c>
@@ -20189,7 +20204,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="395" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A395" s="1" t="s">
         <v>1011</v>
       </c>
@@ -20227,7 +20242,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="396" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A396" s="1" t="s">
         <v>1014</v>
       </c>
@@ -20262,7 +20277,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="397" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A397" s="1" t="s">
         <v>1017</v>
       </c>
@@ -20297,7 +20312,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="398" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A398" s="1" t="s">
         <v>1020</v>
       </c>
@@ -20335,7 +20350,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="399" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A399" s="1" t="s">
         <v>1024</v>
       </c>
@@ -20373,7 +20388,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="400" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A400" s="1" t="s">
         <v>1027</v>
       </c>
@@ -20411,7 +20426,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="401" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A401" s="1" t="s">
         <v>1030</v>
       </c>
@@ -20446,7 +20461,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="402" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A402" s="1" t="s">
         <v>1033</v>
       </c>
@@ -20481,7 +20496,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="403" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A403" s="1" t="s">
         <v>1036</v>
       </c>
@@ -20519,7 +20534,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="404" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A404" s="1" t="s">
         <v>1038</v>
       </c>
@@ -20554,7 +20569,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="405" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A405" s="1" t="s">
         <v>1041</v>
       </c>
@@ -20592,7 +20607,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="406" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A406" s="1" t="s">
         <v>1043</v>
       </c>
@@ -20630,7 +20645,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="407" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A407" s="1" t="s">
         <v>1046</v>
       </c>
@@ -20668,7 +20683,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="408" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A408" s="1" t="s">
         <v>1049</v>
       </c>
@@ -20703,7 +20718,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="409" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A409" s="1" t="s">
         <v>1052</v>
       </c>
@@ -20741,7 +20756,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="410" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A410" s="1" t="s">
         <v>1055</v>
       </c>
@@ -20779,7 +20794,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="411" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A411" s="1" t="s">
         <v>1058</v>
       </c>
@@ -20817,7 +20832,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="412" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A412" s="1" t="s">
         <v>1061</v>
       </c>
@@ -20855,7 +20870,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="413" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A413" s="1" t="s">
         <v>1064</v>
       </c>
@@ -20893,7 +20908,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="414" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A414" s="1" t="s">
         <v>1067</v>
       </c>
@@ -20931,7 +20946,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="415" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A415" s="1" t="s">
         <v>1070</v>
       </c>
@@ -20969,7 +20984,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="416" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A416" s="1" t="s">
         <v>1072</v>
       </c>
@@ -21007,7 +21022,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="417" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A417" s="1" t="s">
         <v>1075</v>
       </c>
@@ -21045,7 +21060,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="418" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A418" s="1" t="s">
         <v>1078</v>
       </c>
@@ -21083,7 +21098,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="419" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A419" s="1" t="s">
         <v>1089</v>
       </c>
@@ -21118,7 +21133,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="420" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A420" s="1" t="s">
         <v>1093</v>
       </c>
@@ -21153,7 +21168,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="421" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A421" s="1" t="s">
         <v>1096</v>
       </c>
@@ -21191,7 +21206,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="422" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A422" s="1" t="s">
         <v>1099</v>
       </c>
@@ -21226,7 +21241,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="423" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A423" s="1" t="s">
         <v>1101</v>
       </c>
@@ -21261,7 +21276,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="424" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A424" s="1" t="s">
         <v>1109</v>
       </c>
@@ -21296,7 +21311,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="425" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A425" s="1" t="s">
         <v>1113</v>
       </c>
@@ -21334,7 +21349,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="426" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A426" s="1" t="s">
         <v>1116</v>
       </c>
@@ -21369,7 +21384,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="427" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A427" s="1" t="s">
         <v>1118</v>
       </c>
@@ -21407,7 +21422,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="428" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A428" s="1" t="s">
         <v>1121</v>
       </c>
@@ -21445,7 +21460,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="429" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A429" s="1" t="s">
         <v>1124</v>
       </c>
@@ -21483,7 +21498,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="430" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A430" s="1" t="s">
         <v>1129</v>
       </c>
@@ -21521,7 +21536,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="431" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A431" s="1" t="s">
         <v>1086</v>
       </c>
@@ -21556,7 +21571,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="432" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A432" s="1" t="s">
         <v>1131</v>
       </c>
@@ -21594,7 +21609,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="433" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A433" s="1" t="s">
         <v>1134</v>
       </c>
@@ -21632,7 +21647,7 @@
         <v>1134</v>
       </c>
     </row>
-    <row r="434" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A434" s="1" t="s">
         <v>1137</v>
       </c>
@@ -21670,7 +21685,7 @@
         <v>1137</v>
       </c>
     </row>
-    <row r="435" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A435" s="1" t="s">
         <v>1140</v>
       </c>
@@ -21708,7 +21723,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="436" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A436" s="1" t="s">
         <v>1143</v>
       </c>
@@ -21746,7 +21761,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="437" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A437" s="1" t="s">
         <v>1145</v>
       </c>
@@ -21781,7 +21796,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="438" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A438" s="1" t="s">
         <v>1149</v>
       </c>
@@ -21819,7 +21834,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="439" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A439" s="1" t="s">
         <v>1152</v>
       </c>
@@ -21854,7 +21869,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="440" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A440" s="1" t="s">
         <v>1155</v>
       </c>
@@ -21892,7 +21907,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="441" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A441" s="1" t="s">
         <v>1157</v>
       </c>
@@ -21927,7 +21942,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="442" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A442" s="1" t="s">
         <v>1161</v>
       </c>
@@ -21962,7 +21977,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="443" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A443" s="1" t="s">
         <v>1164</v>
       </c>
@@ -21997,7 +22012,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="444" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A444" s="1" t="s">
         <v>1167</v>
       </c>
@@ -22032,7 +22047,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="445" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A445" s="1" t="s">
         <v>1171</v>
       </c>
@@ -22067,7 +22082,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="446" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A446" s="1" t="s">
         <v>1174</v>
       </c>
@@ -22102,7 +22117,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="447" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A447" s="1" t="s">
         <v>1179</v>
       </c>
@@ -22140,7 +22155,7 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="448" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A448" s="1" t="s">
         <v>1181</v>
       </c>
@@ -22178,7 +22193,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="449" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A449" s="1" t="s">
         <v>1187</v>
       </c>
@@ -22213,7 +22228,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="450" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A450" s="1" t="s">
         <v>1190</v>
       </c>
@@ -22248,7 +22263,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="451" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A451" s="1" t="s">
         <v>1193</v>
       </c>
@@ -22286,7 +22301,7 @@
         <v>1193</v>
       </c>
     </row>
-    <row r="452" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A452" s="1" t="s">
         <v>1196</v>
       </c>
@@ -22324,7 +22339,7 @@
         <v>1196</v>
       </c>
     </row>
-    <row r="453" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A453" s="1" t="s">
         <v>1199</v>
       </c>
@@ -22359,7 +22374,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="454" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A454" s="1" t="s">
         <v>1202</v>
       </c>
@@ -22397,7 +22412,7 @@
         <v>1202</v>
       </c>
     </row>
-    <row r="455" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A455" s="1" t="s">
         <v>1204</v>
       </c>
@@ -22435,7 +22450,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="456" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A456" s="1" t="s">
         <v>1206</v>
       </c>
@@ -22470,7 +22485,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="457" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A457" s="1" t="s">
         <v>1208</v>
       </c>
@@ -22508,7 +22523,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="458" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A458" s="1" t="s">
         <v>1211</v>
       </c>
@@ -22546,7 +22561,7 @@
         <v>1211</v>
       </c>
     </row>
-    <row r="459" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A459" s="1" t="s">
         <v>1214</v>
       </c>
@@ -22584,7 +22599,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="460" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A460" s="1" t="s">
         <v>1217</v>
       </c>
@@ -22619,7 +22634,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="461" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A461" s="1" t="s">
         <v>1219</v>
       </c>
@@ -22654,7 +22669,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="462" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A462" s="1" t="s">
         <v>1222</v>
       </c>
@@ -22689,7 +22704,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="463" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N463">
         <f>COUNTIF(N2:N462,"*")</f>
         <v>263</v>
@@ -22730,16 +22745,13 @@
     <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="B66" sqref="B66"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="1">
-      <selection activeCell="J72" sqref="J72"/>
-    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
         <v>44903</v>
       </c>
@@ -22747,352 +22759,352 @@
         <v>1496</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>1497</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>1498</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>1499</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>1500</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>1501</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>1502</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>1503</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>1504</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>1505</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>1506</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>1507</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>1508</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>1509</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>1510</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>1511</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>1512</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>1513</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>1514</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>1515</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>1516</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>1517</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>1518</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>1519</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>1520</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>1521</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>1522</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>1523</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>1533</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>1534</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>1535</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>1536</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>1535</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>1537</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>1538</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>1535</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>1539</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>1540</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>1541</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>1535</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>1542</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>1543</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>1535</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>1544</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>1545</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>1535</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>1546</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>1535</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>1547</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>1548</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>1549</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>1551</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>1552</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>1553</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>1554</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>1555</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>1556</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>1557</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>1558</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>1559</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>1560</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>1561</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>1562</v>
       </c>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>1563</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>1564</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>1565</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>1566</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>1567</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>1568</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>1569</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>1570</v>
       </c>

</xml_diff>

<commit_message>
parsed modules spreadsheet - noted additon of depot-tools
</commit_message>
<xml_diff>
--- a/parsed_modules.xlsx
+++ b/parsed_modules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/ucapcjg_ucl_ac_uk/Documents/Work/GitHubRepos/hpc-spack/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:40009_{763C7209-7DDC-4B1B-B313-E43AE37FF459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37A89742-ABBC-4F85-9783-2EF395E8BA13}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="13_ncr:40009_{763C7209-7DDC-4B1B-B313-E43AE37FF459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18FBFE79-9E30-40E6-BF85-9DF1466E3576}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5437" uniqueCount="1573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5439" uniqueCount="1574">
   <si>
     <t>package</t>
   </si>
@@ -4753,6 +4753,9 @@
   </si>
   <si>
     <t>1.11.1.1208</t>
+  </si>
+  <si>
+    <t>pakage made</t>
   </si>
 </sst>
 </file>
@@ -5649,9 +5652,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A281" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A296" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q298" sqref="Q298"/>
+      <selection pane="topRight" activeCell="S299" sqref="S299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -16658,6 +16661,15 @@
       </c>
       <c r="L299" t="s">
         <v>12</v>
+      </c>
+      <c r="P299" t="s">
+        <v>1573</v>
+      </c>
+      <c r="Q299" t="s">
+        <v>1288</v>
+      </c>
+      <c r="R299">
+        <v>4147</v>
       </c>
     </row>
     <row r="300" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
new nedit package added to modules spreadsheet
</commit_message>
<xml_diff>
--- a/parsed_modules.xlsx
+++ b/parsed_modules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/ucapcjg_ucl_ac_uk/Documents/Work/GitHubRepos/hpc-spack/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="13_ncr:40009_{763C7209-7DDC-4B1B-B313-E43AE37FF459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18FBFE79-9E30-40E6-BF85-9DF1466E3576}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="13_ncr:40009_{763C7209-7DDC-4B1B-B313-E43AE37FF459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79D82A47-2A06-4EF4-AA09-DAB4F7F6C9D1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="20928" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parsed_modules" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5439" uniqueCount="1574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5447" uniqueCount="1580">
   <si>
     <t>package</t>
   </si>
@@ -4756,13 +4756,31 @@
   </si>
   <si>
     <t>pakage made</t>
+  </si>
+  <si>
+    <t>Haskell Platform is deprecated!!</t>
+  </si>
+  <si>
+    <t>LATER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://get-ghcup.haskell.org is long insteractive install script </t>
+  </si>
+  <si>
+    <t>Package choices: java · Issue #14 · UCL-ARC/hpc-spack (github.com)</t>
+  </si>
+  <si>
+    <t>package made</t>
+  </si>
+  <si>
+    <t>download is at https://ccl.northwestern.edu/netlogo/6.3.0/NetLogo-6.3.0-64.tgz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4900,6 +4918,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -5208,7 +5234,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -5251,8 +5277,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -5263,8 +5290,9 @@
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -5298,6 +5326,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -5351,6 +5380,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5652,31 +5685,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A296" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A311" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S299" sqref="S299"/>
+      <selection pane="topRight" activeCell="O322" sqref="O322"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="29.28515625" style="1" customWidth="1"/>
-    <col min="9" max="10" width="15.42578125" customWidth="1"/>
-    <col min="11" max="11" width="49.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.54296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.26953125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.26953125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.26953125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23.54296875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="29.26953125" style="1" customWidth="1"/>
+    <col min="9" max="10" width="15.453125" customWidth="1"/>
+    <col min="11" max="11" width="49.54296875" customWidth="1"/>
     <col min="12" max="12" width="17" customWidth="1"/>
-    <col min="13" max="13" width="6.28515625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="16.7109375" customWidth="1"/>
-    <col min="15" max="15" width="22.28515625" customWidth="1"/>
-    <col min="16" max="16" width="20.5703125" customWidth="1"/>
+    <col min="13" max="13" width="6.26953125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="16.7265625" customWidth="1"/>
+    <col min="15" max="15" width="22.26953125" customWidth="1"/>
+    <col min="16" max="16" width="20.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5717,7 +5750,7 @@
         <v>1494</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>43</v>
       </c>
@@ -5752,7 +5785,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
@@ -5790,7 +5823,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>53</v>
       </c>
@@ -5828,7 +5861,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>56</v>
       </c>
@@ -5863,7 +5896,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>59</v>
       </c>
@@ -5901,7 +5934,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>64</v>
       </c>
@@ -5936,7 +5969,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>67</v>
       </c>
@@ -5974,7 +6007,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>70</v>
       </c>
@@ -6009,7 +6042,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>73</v>
       </c>
@@ -6047,7 +6080,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>76</v>
       </c>
@@ -6082,7 +6115,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>79</v>
       </c>
@@ -6117,7 +6150,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>82</v>
       </c>
@@ -6155,7 +6188,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>85</v>
       </c>
@@ -6193,7 +6226,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>88</v>
       </c>
@@ -6228,7 +6261,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>91</v>
       </c>
@@ -6266,7 +6299,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>94</v>
       </c>
@@ -6301,7 +6334,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>97</v>
       </c>
@@ -6336,7 +6369,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>100</v>
       </c>
@@ -6371,7 +6404,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>103</v>
       </c>
@@ -6406,7 +6439,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>106</v>
       </c>
@@ -6441,7 +6474,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>109</v>
       </c>
@@ -6476,7 +6509,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>112</v>
       </c>
@@ -6511,7 +6544,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>116</v>
       </c>
@@ -6549,7 +6582,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>119</v>
       </c>
@@ -6587,7 +6620,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>122</v>
       </c>
@@ -6625,7 +6658,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>125</v>
       </c>
@@ -6663,7 +6696,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>136</v>
       </c>
@@ -6698,7 +6731,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>140</v>
       </c>
@@ -6736,7 +6769,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>143</v>
       </c>
@@ -6774,7 +6807,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>147</v>
       </c>
@@ -6809,7 +6842,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>150</v>
       </c>
@@ -6844,7 +6877,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>154</v>
       </c>
@@ -6879,7 +6912,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>157</v>
       </c>
@@ -6914,7 +6947,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>162</v>
       </c>
@@ -6952,7 +6985,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>165</v>
       </c>
@@ -6987,7 +7020,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>168</v>
       </c>
@@ -7022,7 +7055,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>171</v>
       </c>
@@ -7057,7 +7090,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>174</v>
       </c>
@@ -7092,7 +7125,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>177</v>
       </c>
@@ -7127,7 +7160,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>180</v>
       </c>
@@ -7162,7 +7195,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>183</v>
       </c>
@@ -7197,7 +7230,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>187</v>
       </c>
@@ -7235,7 +7268,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>193</v>
       </c>
@@ -7273,7 +7306,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>197</v>
       </c>
@@ -7308,7 +7341,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>200</v>
       </c>
@@ -7343,7 +7376,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>202</v>
       </c>
@@ -7381,7 +7414,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>205</v>
       </c>
@@ -7419,7 +7452,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>208</v>
       </c>
@@ -7457,7 +7490,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>211</v>
       </c>
@@ -7495,7 +7528,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>216</v>
       </c>
@@ -7533,7 +7566,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>219</v>
       </c>
@@ -7568,7 +7601,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>222</v>
       </c>
@@ -7603,7 +7636,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>226</v>
       </c>
@@ -7641,7 +7674,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>230</v>
       </c>
@@ -7676,7 +7709,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>233</v>
       </c>
@@ -7711,7 +7744,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>239</v>
       </c>
@@ -7749,7 +7782,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>246</v>
       </c>
@@ -7787,7 +7820,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>249</v>
       </c>
@@ -7825,7 +7858,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>252</v>
       </c>
@@ -7860,7 +7893,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>258</v>
       </c>
@@ -7895,7 +7928,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>255</v>
       </c>
@@ -7933,7 +7966,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>261</v>
       </c>
@@ -7968,7 +8001,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>264</v>
       </c>
@@ -8006,7 +8039,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>268</v>
       </c>
@@ -8044,7 +8077,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>272</v>
       </c>
@@ -8079,7 +8112,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>275</v>
       </c>
@@ -8114,7 +8147,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>278</v>
       </c>
@@ -8152,7 +8185,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>281</v>
       </c>
@@ -8190,7 +8223,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>284</v>
       </c>
@@ -8228,7 +8261,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>287</v>
       </c>
@@ -8266,7 +8299,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>290</v>
       </c>
@@ -8304,7 +8337,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>292</v>
       </c>
@@ -8339,7 +8372,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>295</v>
       </c>
@@ -8377,7 +8410,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>298</v>
       </c>
@@ -8412,7 +8445,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>301</v>
       </c>
@@ -8450,7 +8483,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>304</v>
       </c>
@@ -8488,7 +8521,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>309</v>
       </c>
@@ -8523,7 +8556,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>312</v>
       </c>
@@ -8561,7 +8594,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>315</v>
       </c>
@@ -8599,7 +8632,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>319</v>
       </c>
@@ -8637,7 +8670,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>322</v>
       </c>
@@ -8675,7 +8708,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>325</v>
       </c>
@@ -8710,7 +8743,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>328</v>
       </c>
@@ -8748,7 +8781,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>331</v>
       </c>
@@ -8786,7 +8819,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>338</v>
       </c>
@@ -8824,7 +8857,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>341</v>
       </c>
@@ -8862,7 +8895,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>344</v>
       </c>
@@ -8900,7 +8933,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="89" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>347</v>
       </c>
@@ -8938,7 +8971,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>350</v>
       </c>
@@ -8976,7 +9009,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>353</v>
       </c>
@@ -9014,7 +9047,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>362</v>
       </c>
@@ -9052,7 +9085,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>365</v>
       </c>
@@ -9090,7 +9123,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
         <v>368</v>
       </c>
@@ -9125,7 +9158,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>371</v>
       </c>
@@ -9160,7 +9193,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
         <v>374</v>
       </c>
@@ -9198,7 +9231,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>377</v>
       </c>
@@ -9233,7 +9266,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
         <v>380</v>
       </c>
@@ -9271,7 +9304,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
         <v>383</v>
       </c>
@@ -9306,7 +9339,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
         <v>387</v>
       </c>
@@ -9341,7 +9374,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
         <v>390</v>
       </c>
@@ -9379,7 +9412,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="102" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
         <v>393</v>
       </c>
@@ -9414,7 +9447,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>396</v>
       </c>
@@ -9452,7 +9485,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="104" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>399</v>
       </c>
@@ -9487,7 +9520,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
         <v>402</v>
       </c>
@@ -9525,7 +9558,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="106" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>405</v>
       </c>
@@ -9560,7 +9593,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
         <v>408</v>
       </c>
@@ -9598,7 +9631,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="108" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
         <v>414</v>
       </c>
@@ -9636,7 +9669,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
         <v>418</v>
       </c>
@@ -9674,7 +9707,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="110" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
         <v>421</v>
       </c>
@@ -9709,7 +9742,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
         <v>424</v>
       </c>
@@ -9744,7 +9777,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
         <v>427</v>
       </c>
@@ -9779,7 +9812,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="113" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
         <v>430</v>
       </c>
@@ -9817,7 +9850,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="114" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
         <v>437</v>
       </c>
@@ -9855,7 +9888,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="115" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
         <v>440</v>
       </c>
@@ -9893,7 +9926,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="116" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
         <v>443</v>
       </c>
@@ -9931,7 +9964,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="117" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
         <v>447</v>
       </c>
@@ -9969,7 +10002,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="118" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
         <v>450</v>
       </c>
@@ -10007,7 +10040,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
         <v>454</v>
       </c>
@@ -10045,7 +10078,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
         <v>457</v>
       </c>
@@ -10080,7 +10113,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="121" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
         <v>460</v>
       </c>
@@ -10115,7 +10148,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="122" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
         <v>463</v>
       </c>
@@ -10153,7 +10186,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="123" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
         <v>466</v>
       </c>
@@ -10188,7 +10221,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="124" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
         <v>470</v>
       </c>
@@ -10223,7 +10256,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="125" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
         <v>473</v>
       </c>
@@ -10261,7 +10294,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="126" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
         <v>477</v>
       </c>
@@ -10296,7 +10329,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="127" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
         <v>482</v>
       </c>
@@ -10334,7 +10367,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="128" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
         <v>486</v>
       </c>
@@ -10369,7 +10402,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="129" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
         <v>490</v>
       </c>
@@ -10404,7 +10437,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="130" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
         <v>493</v>
       </c>
@@ -10442,7 +10475,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="131" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
         <v>497</v>
       </c>
@@ -10480,7 +10513,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="132" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
         <v>500</v>
       </c>
@@ -10518,7 +10551,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="133" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
         <v>503</v>
       </c>
@@ -10553,7 +10586,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="134" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
         <v>506</v>
       </c>
@@ -10591,7 +10624,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="135" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
         <v>512</v>
       </c>
@@ -10629,7 +10662,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="136" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
         <v>515</v>
       </c>
@@ -10667,7 +10700,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="137" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
         <v>522</v>
       </c>
@@ -10702,7 +10735,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="138" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
         <v>525</v>
       </c>
@@ -10737,7 +10770,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="139" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
         <v>528</v>
       </c>
@@ -10772,7 +10805,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="140" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
         <v>531</v>
       </c>
@@ -10807,7 +10840,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="141" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
         <v>534</v>
       </c>
@@ -10845,7 +10878,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="142" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
         <v>539</v>
       </c>
@@ -10880,7 +10913,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="143" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
         <v>546</v>
       </c>
@@ -10918,7 +10951,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="144" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
         <v>550</v>
       </c>
@@ -10956,7 +10989,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="145" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
         <v>553</v>
       </c>
@@ -10994,7 +11027,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="146" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
         <v>556</v>
       </c>
@@ -11032,7 +11065,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="147" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
         <v>560</v>
       </c>
@@ -11067,7 +11100,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
         <v>564</v>
       </c>
@@ -11105,7 +11138,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="149" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
         <v>568</v>
       </c>
@@ -11143,7 +11176,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="150" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
         <v>571</v>
       </c>
@@ -11178,7 +11211,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="151" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
         <v>574</v>
       </c>
@@ -11216,7 +11249,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="152" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
         <v>578</v>
       </c>
@@ -11254,7 +11287,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="153" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
         <v>581</v>
       </c>
@@ -11292,7 +11325,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="154" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
         <v>584</v>
       </c>
@@ -11330,7 +11363,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="155" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
         <v>587</v>
       </c>
@@ -11368,7 +11401,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="156" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
         <v>590</v>
       </c>
@@ -11403,7 +11436,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="157" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
         <v>593</v>
       </c>
@@ -11441,7 +11474,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="158" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
         <v>596</v>
       </c>
@@ -11476,7 +11509,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="159" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
         <v>599</v>
       </c>
@@ -11511,7 +11544,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="160" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
         <v>602</v>
       </c>
@@ -11549,7 +11582,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="161" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
         <v>605</v>
       </c>
@@ -11587,7 +11620,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="162" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
         <v>610</v>
       </c>
@@ -11625,7 +11658,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="163" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
         <v>614</v>
       </c>
@@ -11663,7 +11696,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="164" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
         <v>618</v>
       </c>
@@ -11698,7 +11731,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="165" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
         <v>621</v>
       </c>
@@ -11736,7 +11769,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="166" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
         <v>624</v>
       </c>
@@ -11774,7 +11807,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="167" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
         <v>627</v>
       </c>
@@ -11809,7 +11842,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="168" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
         <v>630</v>
       </c>
@@ -11844,7 +11877,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="169" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
         <v>633</v>
       </c>
@@ -11879,7 +11912,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="170" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
         <v>636</v>
       </c>
@@ -11914,7 +11947,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="171" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
         <v>639</v>
       </c>
@@ -11949,7 +11982,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="172" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A172" s="1" t="s">
         <v>642</v>
       </c>
@@ -11984,7 +12017,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="173" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A173" s="1" t="s">
         <v>645</v>
       </c>
@@ -12019,7 +12052,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="174" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
         <v>648</v>
       </c>
@@ -12057,7 +12090,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="175" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A175" s="1" t="s">
         <v>659</v>
       </c>
@@ -12095,7 +12128,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="176" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A176" s="1" t="s">
         <v>662</v>
       </c>
@@ -12133,7 +12166,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="177" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" s="1" t="s">
         <v>665</v>
       </c>
@@ -12168,7 +12201,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="178" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A178" s="1" t="s">
         <v>667</v>
       </c>
@@ -12206,7 +12239,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="179" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A179" s="1" t="s">
         <v>672</v>
       </c>
@@ -12241,7 +12274,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="180" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A180" s="1" t="s">
         <v>677</v>
       </c>
@@ -12279,7 +12312,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="181" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A181" s="1" t="s">
         <v>680</v>
       </c>
@@ -12314,7 +12347,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="182" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" s="1" t="s">
         <v>682</v>
       </c>
@@ -12349,7 +12382,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="183" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" s="1" t="s">
         <v>685</v>
       </c>
@@ -12387,7 +12420,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="184" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A184" s="1" t="s">
         <v>688</v>
       </c>
@@ -12425,7 +12458,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="185" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A185" s="1" t="s">
         <v>692</v>
       </c>
@@ -12463,7 +12496,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="186" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A186" s="1" t="s">
         <v>695</v>
       </c>
@@ -12498,7 +12531,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="187" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A187" s="1" t="s">
         <v>699</v>
       </c>
@@ -12536,7 +12569,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="188" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A188" s="1" t="s">
         <v>702</v>
       </c>
@@ -12571,7 +12604,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="189" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A189" s="1" t="s">
         <v>705</v>
       </c>
@@ -12606,7 +12639,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="190" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A190" s="1" t="s">
         <v>708</v>
       </c>
@@ -12644,7 +12677,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="191" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A191" s="1" t="s">
         <v>711</v>
       </c>
@@ -12679,7 +12712,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="192" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A192" s="1" t="s">
         <v>714</v>
       </c>
@@ -12717,7 +12750,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="193" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A193" s="1" t="s">
         <v>717</v>
       </c>
@@ -12752,7 +12785,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="194" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A194" s="1" t="s">
         <v>721</v>
       </c>
@@ -12790,7 +12823,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="195" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A195" s="1" t="s">
         <v>724</v>
       </c>
@@ -12825,7 +12858,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="196" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A196" s="1" t="s">
         <v>727</v>
       </c>
@@ -12860,7 +12893,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="197" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A197" s="1" t="s">
         <v>730</v>
       </c>
@@ -12898,7 +12931,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="198" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A198" s="1" t="s">
         <v>734</v>
       </c>
@@ -12933,7 +12966,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="199" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A199" s="1" t="s">
         <v>737</v>
       </c>
@@ -12971,7 +13004,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="200" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A200" s="1" t="s">
         <v>740</v>
       </c>
@@ -13009,7 +13042,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="201" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A201" s="1" t="s">
         <v>743</v>
       </c>
@@ -13047,7 +13080,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="202" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A202" s="1" t="s">
         <v>746</v>
       </c>
@@ -13082,7 +13115,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="203" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A203" s="1" t="s">
         <v>749</v>
       </c>
@@ -13117,7 +13150,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="204" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A204" s="1" t="s">
         <v>752</v>
       </c>
@@ -13155,7 +13188,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="205" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A205" s="1" t="s">
         <v>755</v>
       </c>
@@ -13190,7 +13223,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="206" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A206" s="1" t="s">
         <v>758</v>
       </c>
@@ -13225,7 +13258,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="207" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A207" s="1" t="s">
         <v>761</v>
       </c>
@@ -13260,7 +13293,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="208" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A208" s="1" t="s">
         <v>767</v>
       </c>
@@ -13295,7 +13328,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="209" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A209" s="1" t="s">
         <v>771</v>
       </c>
@@ -13333,7 +13366,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="210" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A210" s="1" t="s">
         <v>774</v>
       </c>
@@ -13377,7 +13410,7 @@
         <v>1528</v>
       </c>
     </row>
-    <row r="211" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A211" s="1" t="s">
         <v>777</v>
       </c>
@@ -13415,7 +13448,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="212" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A212" s="1" t="s">
         <v>780</v>
       </c>
@@ -13450,7 +13483,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="213" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A213" s="1" t="s">
         <v>783</v>
       </c>
@@ -13488,7 +13521,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="214" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A214" s="1" t="s">
         <v>786</v>
       </c>
@@ -13526,7 +13559,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="215" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A215" s="1" t="s">
         <v>788</v>
       </c>
@@ -13564,7 +13597,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="216" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A216" s="1" t="s">
         <v>791</v>
       </c>
@@ -13599,7 +13632,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="217" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A217" s="1" t="s">
         <v>793</v>
       </c>
@@ -13637,7 +13670,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="218" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A218" s="1" t="s">
         <v>796</v>
       </c>
@@ -13672,7 +13705,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="219" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A219" s="1" t="s">
         <v>799</v>
       </c>
@@ -13710,7 +13743,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="220" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A220" s="1" t="s">
         <v>802</v>
       </c>
@@ -13748,7 +13781,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="221" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A221" s="1" t="s">
         <v>806</v>
       </c>
@@ -13783,7 +13816,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="222" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A222" s="1" t="s">
         <v>809</v>
       </c>
@@ -13821,7 +13854,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="223" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A223" s="1" t="s">
         <v>812</v>
       </c>
@@ -13859,7 +13892,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="224" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A224" s="1" t="s">
         <v>815</v>
       </c>
@@ -13897,7 +13930,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="225" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A225" s="1" t="s">
         <v>821</v>
       </c>
@@ -13935,7 +13968,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="226" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A226" s="1" t="s">
         <v>824</v>
       </c>
@@ -13973,7 +14006,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="227" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A227" s="1" t="s">
         <v>827</v>
       </c>
@@ -14008,7 +14041,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="228" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A228" s="1" t="s">
         <v>830</v>
       </c>
@@ -14046,7 +14079,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="229" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A229" s="1" t="s">
         <v>834</v>
       </c>
@@ -14081,7 +14114,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="230" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A230" s="1" t="s">
         <v>837</v>
       </c>
@@ -14119,7 +14152,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="231" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A231" s="1" t="s">
         <v>840</v>
       </c>
@@ -14154,7 +14187,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="232" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A232" s="1" t="s">
         <v>842</v>
       </c>
@@ -14192,7 +14225,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="233" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A233" s="1" t="s">
         <v>845</v>
       </c>
@@ -14230,7 +14263,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="234" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A234" s="1" t="s">
         <v>849</v>
       </c>
@@ -14268,7 +14301,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="235" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A235" s="1" t="s">
         <v>852</v>
       </c>
@@ -14303,7 +14336,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="236" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A236" s="1" t="s">
         <v>855</v>
       </c>
@@ -14338,7 +14371,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="237" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A237" s="1" t="s">
         <v>858</v>
       </c>
@@ -14373,7 +14406,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="238" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A238" s="1" t="s">
         <v>861</v>
       </c>
@@ -14411,7 +14444,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="239" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A239" s="1" t="s">
         <v>1445</v>
       </c>
@@ -14446,7 +14479,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="240" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A240" s="1" t="s">
         <v>1447</v>
       </c>
@@ -14481,7 +14514,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="241" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A241" s="1" t="s">
         <v>1449</v>
       </c>
@@ -14516,7 +14549,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="242" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A242" s="1" t="s">
         <v>1450</v>
       </c>
@@ -14551,7 +14584,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="243" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A243" s="1" t="s">
         <v>129</v>
       </c>
@@ -14586,7 +14619,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="244" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A244" s="1" t="s">
         <v>1452</v>
       </c>
@@ -14621,7 +14654,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="245" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A245" s="1" t="s">
         <v>1454</v>
       </c>
@@ -14656,7 +14689,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="246" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A246" s="1" t="s">
         <v>1456</v>
       </c>
@@ -14691,7 +14724,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="247" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A247" s="1" t="s">
         <v>1458</v>
       </c>
@@ -14726,7 +14759,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="248" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A248" s="1" t="s">
         <v>1461</v>
       </c>
@@ -14761,7 +14794,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="249" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A249" s="1" t="s">
         <v>1463</v>
       </c>
@@ -14796,7 +14829,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="250" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A250" s="1" t="s">
         <v>1465</v>
       </c>
@@ -14831,7 +14864,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="251" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A251" s="1" t="s">
         <v>1467</v>
       </c>
@@ -14866,7 +14899,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="252" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A252" s="1" t="s">
         <v>335</v>
       </c>
@@ -14904,7 +14937,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="253" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A253" s="1" t="s">
         <v>1469</v>
       </c>
@@ -14939,7 +14972,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="254" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A254" s="1" t="s">
         <v>1471</v>
       </c>
@@ -14974,7 +15007,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="255" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A255" s="1" t="s">
         <v>543</v>
       </c>
@@ -15012,7 +15045,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="256" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A256" s="1" t="s">
         <v>1476</v>
       </c>
@@ -15047,7 +15080,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="257" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A257" s="1" t="s">
         <v>1478</v>
       </c>
@@ -15082,7 +15115,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="258" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A258" s="1" t="s">
         <v>1378</v>
       </c>
@@ -15117,7 +15150,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="259" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A259" s="1" t="s">
         <v>1480</v>
       </c>
@@ -15152,7 +15185,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="260" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A260" s="1" t="s">
         <v>1482</v>
       </c>
@@ -15187,7 +15220,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="261" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A261" s="1" t="s">
         <v>654</v>
       </c>
@@ -15225,7 +15258,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="262" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A262" s="1" t="s">
         <v>1486</v>
       </c>
@@ -15260,7 +15293,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="263" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A263" s="1" t="s">
         <v>1487</v>
       </c>
@@ -15295,7 +15328,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="264" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A264" s="1" t="s">
         <v>1489</v>
       </c>
@@ -15330,7 +15363,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="265" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A265" s="1" t="s">
         <v>1491</v>
       </c>
@@ -15365,7 +15398,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="266" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A266" s="1" t="s">
         <v>1224</v>
       </c>
@@ -15400,7 +15433,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="267" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A267" s="1" t="s">
         <v>1227</v>
       </c>
@@ -15435,7 +15468,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="268" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A268" s="1" t="s">
         <v>1229</v>
       </c>
@@ -15473,7 +15506,7 @@
         <v>1229</v>
       </c>
     </row>
-    <row r="269" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A269" s="1" t="s">
         <v>1081</v>
       </c>
@@ -15511,7 +15544,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="270" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A270" s="1" t="s">
         <v>1105</v>
       </c>
@@ -15549,7 +15582,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="271" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A271" s="1" t="s">
         <v>1232</v>
       </c>
@@ -15584,7 +15617,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="272" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A272" s="1" t="s">
         <v>1236</v>
       </c>
@@ -15622,7 +15655,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="273" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A273" s="1" t="s">
         <v>1241</v>
       </c>
@@ -15660,7 +15693,7 @@
         <v>1241</v>
       </c>
     </row>
-    <row r="274" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A274" s="1" t="s">
         <v>11</v>
       </c>
@@ -15695,7 +15728,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="275" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A275" s="1" t="s">
         <v>15</v>
       </c>
@@ -15730,7 +15763,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="276" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A276" s="1" t="s">
         <v>18</v>
       </c>
@@ -15765,7 +15798,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="277" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A277" s="1" t="s">
         <v>21</v>
       </c>
@@ -15800,7 +15833,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="278" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A278" s="1" t="s">
         <v>24</v>
       </c>
@@ -15835,7 +15868,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="279" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A279" s="1" t="s">
         <v>27</v>
       </c>
@@ -15873,7 +15906,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="280" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A280" s="1" t="s">
         <v>30</v>
       </c>
@@ -15908,7 +15941,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="281" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A281" s="1" t="s">
         <v>32</v>
       </c>
@@ -15946,7 +15979,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="282" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A282" s="1" t="s">
         <v>35</v>
       </c>
@@ -15984,7 +16017,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="283" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A283" s="1" t="s">
         <v>38</v>
       </c>
@@ -16019,7 +16052,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="284" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A284" s="1" t="s">
         <v>40</v>
       </c>
@@ -16054,7 +16087,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="285" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A285" s="1" t="s">
         <v>1244</v>
       </c>
@@ -16089,7 +16122,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="286" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A286" s="1" t="s">
         <v>1248</v>
       </c>
@@ -16133,7 +16166,7 @@
         <v>2.69</v>
       </c>
     </row>
-    <row r="287" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A287" s="1" t="s">
         <v>1251</v>
       </c>
@@ -16174,7 +16207,7 @@
         <v>1251</v>
       </c>
     </row>
-    <row r="288" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A288" s="1" t="s">
         <v>1254</v>
       </c>
@@ -16221,7 +16254,7 @@
         <v>1524</v>
       </c>
     </row>
-    <row r="289" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A289" s="1" t="s">
         <v>1257</v>
       </c>
@@ -16265,7 +16298,7 @@
         <v>1530</v>
       </c>
     </row>
-    <row r="290" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A290" s="1" t="s">
         <v>1260</v>
       </c>
@@ -16306,7 +16339,7 @@
         <v>2.38</v>
       </c>
     </row>
-    <row r="291" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A291" s="1" t="s">
         <v>1263</v>
       </c>
@@ -16347,7 +16380,7 @@
         <v>1531</v>
       </c>
     </row>
-    <row r="292" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A292" s="1" t="s">
         <v>1266</v>
       </c>
@@ -16388,7 +16421,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="293" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A293" s="1" t="s">
         <v>1269</v>
       </c>
@@ -16432,7 +16465,7 @@
         <v>1572</v>
       </c>
     </row>
-    <row r="294" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A294" s="1" t="s">
         <v>1272</v>
       </c>
@@ -16473,7 +16506,7 @@
         <v>1532</v>
       </c>
     </row>
-    <row r="295" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A295" s="1" t="s">
         <v>1275</v>
       </c>
@@ -16511,7 +16544,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="296" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A296" s="1" t="s">
         <v>1278</v>
       </c>
@@ -16549,7 +16582,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="297" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A297" s="1" t="s">
         <v>1281</v>
       </c>
@@ -16587,7 +16620,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="298" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A298" s="1" t="s">
         <v>1285</v>
       </c>
@@ -16628,7 +16661,7 @@
         <v>1550</v>
       </c>
     </row>
-    <row r="299" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A299" s="1" t="s">
         <v>1288</v>
       </c>
@@ -16672,7 +16705,7 @@
         <v>4147</v>
       </c>
     </row>
-    <row r="300" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A300" s="1" t="s">
         <v>1291</v>
       </c>
@@ -16710,7 +16743,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="301" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A301" s="1" t="s">
         <v>1294</v>
       </c>
@@ -16748,7 +16781,7 @@
         <v>1294</v>
       </c>
     </row>
-    <row r="302" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A302" s="1" t="s">
         <v>1297</v>
       </c>
@@ -16786,7 +16819,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="303" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A303" s="1" t="s">
         <v>1300</v>
       </c>
@@ -16824,7 +16857,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="304" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A304" s="1" t="s">
         <v>1303</v>
       </c>
@@ -16862,7 +16895,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="305" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A305" s="1" t="s">
         <v>1306</v>
       </c>
@@ -16900,7 +16933,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="306" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A306" s="1" t="s">
         <v>1309</v>
       </c>
@@ -16938,7 +16971,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="307" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A307" s="1" t="s">
         <v>1312</v>
       </c>
@@ -16976,7 +17009,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="308" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A308" s="1" t="s">
         <v>1314</v>
       </c>
@@ -17014,7 +17047,7 @@
         <v>1314</v>
       </c>
     </row>
-    <row r="309" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A309" s="1" t="s">
         <v>1317</v>
       </c>
@@ -17048,8 +17081,17 @@
       <c r="L309" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="310" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O309" t="s">
+        <v>1575</v>
+      </c>
+      <c r="P309" t="s">
+        <v>1576</v>
+      </c>
+      <c r="R309" s="6" t="s">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="310" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A310" s="1" t="s">
         <v>1320</v>
       </c>
@@ -17087,7 +17129,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="311" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A311" s="1" t="s">
         <v>1322</v>
       </c>
@@ -17121,8 +17163,14 @@
       <c r="L311" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="312" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O311" t="s">
+        <v>1575</v>
+      </c>
+      <c r="P311" s="6" t="s">
+        <v>1577</v>
+      </c>
+    </row>
+    <row r="312" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A312" s="1" t="s">
         <v>1327</v>
       </c>
@@ -17160,7 +17208,7 @@
         <v>1327</v>
       </c>
     </row>
-    <row r="313" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A313" s="1" t="s">
         <v>1330</v>
       </c>
@@ -17204,7 +17252,7 @@
         <v>1527</v>
       </c>
     </row>
-    <row r="314" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A314" s="1" t="s">
         <v>1333</v>
       </c>
@@ -17242,7 +17290,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="315" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A315" s="1" t="s">
         <v>1336</v>
       </c>
@@ -17280,7 +17328,7 @@
         <v>1336</v>
       </c>
     </row>
-    <row r="316" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A316" s="1" t="s">
         <v>1339</v>
       </c>
@@ -17318,7 +17366,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="317" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A317" s="1" t="s">
         <v>1342</v>
       </c>
@@ -17356,7 +17404,7 @@
         <v>1342</v>
       </c>
     </row>
-    <row r="318" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A318" s="1" t="s">
         <v>1345</v>
       </c>
@@ -17394,7 +17442,7 @@
         <v>1345</v>
       </c>
     </row>
-    <row r="319" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A319" s="1" t="s">
         <v>1348</v>
       </c>
@@ -17432,7 +17480,7 @@
         <v>1348</v>
       </c>
     </row>
-    <row r="320" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A320" s="1" t="s">
         <v>1351</v>
       </c>
@@ -17470,7 +17518,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="321" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A321" s="1" t="s">
         <v>1354</v>
       </c>
@@ -17504,8 +17552,17 @@
       <c r="L321" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="322" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P321" t="s">
+        <v>1578</v>
+      </c>
+      <c r="Q321" t="s">
+        <v>1354</v>
+      </c>
+      <c r="R321">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="322" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A322" s="1" t="s">
         <v>1357</v>
       </c>
@@ -17539,8 +17596,11 @@
       <c r="L322" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="323" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O322" t="s">
+        <v>1579</v>
+      </c>
+    </row>
+    <row r="323" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A323" s="1" t="s">
         <v>1360</v>
       </c>
@@ -17578,7 +17638,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="324" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A324" s="1" t="s">
         <v>1363</v>
       </c>
@@ -17616,7 +17676,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="325" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A325" s="1" t="s">
         <v>1366</v>
       </c>
@@ -17651,7 +17711,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="326" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A326" s="1" t="s">
         <v>1369</v>
       </c>
@@ -17689,7 +17749,7 @@
         <v>1369</v>
       </c>
     </row>
-    <row r="327" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A327" s="1" t="s">
         <v>1372</v>
       </c>
@@ -17730,7 +17790,7 @@
         <v>1529</v>
       </c>
     </row>
-    <row r="328" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A328" s="1" t="s">
         <v>1375</v>
       </c>
@@ -17765,7 +17825,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="329" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A329" s="1" t="s">
         <v>1383</v>
       </c>
@@ -17803,7 +17863,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="330" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A330" s="1" t="s">
         <v>1388</v>
       </c>
@@ -17841,7 +17901,7 @@
         <v>1388</v>
       </c>
     </row>
-    <row r="331" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A331" s="1" t="s">
         <v>1391</v>
       </c>
@@ -17879,7 +17939,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="332" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A332" s="1" t="s">
         <v>1394</v>
       </c>
@@ -17917,7 +17977,7 @@
         <v>1394</v>
       </c>
     </row>
-    <row r="333" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A333" s="1" t="s">
         <v>1397</v>
       </c>
@@ -17952,7 +18012,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="334" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A334" s="1" t="s">
         <v>1400</v>
       </c>
@@ -17987,7 +18047,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="335" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A335" s="1" t="s">
         <v>1403</v>
       </c>
@@ -18025,7 +18085,7 @@
         <v>1403</v>
       </c>
     </row>
-    <row r="336" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A336" s="1" t="s">
         <v>1406</v>
       </c>
@@ -18060,7 +18120,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="337" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A337" s="1" t="s">
         <v>1409</v>
       </c>
@@ -18095,7 +18155,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="338" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A338" s="1" t="s">
         <v>1412</v>
       </c>
@@ -18133,7 +18193,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="339" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A339" s="1" t="s">
         <v>1415</v>
       </c>
@@ -18171,7 +18231,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="340" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A340" s="1" t="s">
         <v>1418</v>
       </c>
@@ -18209,7 +18269,7 @@
         <v>1418</v>
       </c>
     </row>
-    <row r="341" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A341" s="1" t="s">
         <v>1421</v>
       </c>
@@ -18247,7 +18307,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="342" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A342" s="1" t="s">
         <v>1424</v>
       </c>
@@ -18285,7 +18345,7 @@
         <v>1424</v>
       </c>
     </row>
-    <row r="343" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A343" s="1" t="s">
         <v>1427</v>
       </c>
@@ -18323,7 +18383,7 @@
         <v>1427</v>
       </c>
     </row>
-    <row r="344" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A344" s="1" t="s">
         <v>1430</v>
       </c>
@@ -18361,7 +18421,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="345" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A345" s="1" t="s">
         <v>1433</v>
       </c>
@@ -18396,7 +18456,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="346" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A346" s="1" t="s">
         <v>1436</v>
       </c>
@@ -18434,7 +18494,7 @@
         <v>1436</v>
       </c>
     </row>
-    <row r="347" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A347" s="1" t="s">
         <v>1439</v>
       </c>
@@ -18469,7 +18529,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="348" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A348" s="1" t="s">
         <v>1442</v>
       </c>
@@ -18504,7 +18564,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="349" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A349" s="1" t="s">
         <v>864</v>
       </c>
@@ -18542,7 +18602,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="350" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A350" s="1" t="s">
         <v>867</v>
       </c>
@@ -18580,7 +18640,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="351" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A351" s="1" t="s">
         <v>870</v>
       </c>
@@ -18618,7 +18678,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="352" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A352" s="1" t="s">
         <v>873</v>
       </c>
@@ -18656,7 +18716,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="353" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A353" s="1" t="s">
         <v>876</v>
       </c>
@@ -18694,7 +18754,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="354" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A354" s="1" t="s">
         <v>882</v>
       </c>
@@ -18732,7 +18792,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="355" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A355" s="1" t="s">
         <v>885</v>
       </c>
@@ -18767,7 +18827,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="356" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A356" s="1" t="s">
         <v>888</v>
       </c>
@@ -18805,7 +18865,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="357" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A357" s="1" t="s">
         <v>894</v>
       </c>
@@ -18840,7 +18900,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="358" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A358" s="1" t="s">
         <v>897</v>
       </c>
@@ -18878,7 +18938,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="359" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A359" s="1" t="s">
         <v>900</v>
       </c>
@@ -18916,7 +18976,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="360" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A360" s="1" t="s">
         <v>903</v>
       </c>
@@ -18951,7 +19011,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="361" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A361" s="1" t="s">
         <v>906</v>
       </c>
@@ -18989,7 +19049,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="362" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A362" s="1" t="s">
         <v>909</v>
       </c>
@@ -19027,7 +19087,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="363" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A363" s="1" t="s">
         <v>912</v>
       </c>
@@ -19062,7 +19122,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="364" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A364" s="1" t="s">
         <v>914</v>
       </c>
@@ -19100,7 +19160,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="365" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A365" s="1" t="s">
         <v>917</v>
       </c>
@@ -19138,7 +19198,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="366" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A366" s="1" t="s">
         <v>920</v>
       </c>
@@ -19176,7 +19236,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="367" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A367" s="1" t="s">
         <v>923</v>
       </c>
@@ -19214,7 +19274,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="368" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A368" s="1" t="s">
         <v>930</v>
       </c>
@@ -19249,7 +19309,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="369" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A369" s="1" t="s">
         <v>932</v>
       </c>
@@ -19287,7 +19347,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="370" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A370" s="1" t="s">
         <v>935</v>
       </c>
@@ -19325,7 +19385,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="371" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A371" s="1" t="s">
         <v>938</v>
       </c>
@@ -19360,7 +19420,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="372" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A372" s="1" t="s">
         <v>943</v>
       </c>
@@ -19395,7 +19455,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="373" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A373" s="1" t="s">
         <v>946</v>
       </c>
@@ -19433,7 +19493,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="374" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A374" s="1" t="s">
         <v>948</v>
       </c>
@@ -19471,7 +19531,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="375" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A375" s="1" t="s">
         <v>950</v>
       </c>
@@ -19509,7 +19569,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="376" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A376" s="1" t="s">
         <v>953</v>
       </c>
@@ -19544,7 +19604,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="377" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A377" s="1" t="s">
         <v>955</v>
       </c>
@@ -19582,7 +19642,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="378" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A378" s="1" t="s">
         <v>958</v>
       </c>
@@ -19620,7 +19680,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="379" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A379" s="1" t="s">
         <v>961</v>
       </c>
@@ -19658,7 +19718,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="380" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A380" s="1" t="s">
         <v>964</v>
       </c>
@@ -19696,7 +19756,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="381" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A381" s="1" t="s">
         <v>967</v>
       </c>
@@ -19734,7 +19794,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="382" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A382" s="1" t="s">
         <v>970</v>
       </c>
@@ -19769,7 +19829,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="383" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A383" s="1" t="s">
         <v>357</v>
       </c>
@@ -19804,7 +19864,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="384" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A384" s="1" t="s">
         <v>973</v>
       </c>
@@ -19839,7 +19899,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="385" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A385" s="1" t="s">
         <v>977</v>
       </c>
@@ -19877,7 +19937,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="386" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A386" s="1" t="s">
         <v>980</v>
       </c>
@@ -19915,7 +19975,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="387" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A387" s="1" t="s">
         <v>986</v>
       </c>
@@ -19953,7 +20013,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="388" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A388" s="1" t="s">
         <v>989</v>
       </c>
@@ -19991,7 +20051,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="389" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A389" s="1" t="s">
         <v>992</v>
       </c>
@@ -20029,7 +20089,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="390" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A390" s="1" t="s">
         <v>996</v>
       </c>
@@ -20067,7 +20127,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="391" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A391" s="1" t="s">
         <v>999</v>
       </c>
@@ -20105,7 +20165,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="392" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A392" s="1" t="s">
         <v>1002</v>
       </c>
@@ -20143,7 +20203,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="393" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A393" s="1" t="s">
         <v>1005</v>
       </c>
@@ -20178,7 +20238,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="394" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A394" s="1" t="s">
         <v>1008</v>
       </c>
@@ -20216,7 +20276,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="395" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A395" s="1" t="s">
         <v>1011</v>
       </c>
@@ -20254,7 +20314,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="396" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A396" s="1" t="s">
         <v>1014</v>
       </c>
@@ -20289,7 +20349,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="397" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A397" s="1" t="s">
         <v>1017</v>
       </c>
@@ -20324,7 +20384,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="398" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A398" s="1" t="s">
         <v>1020</v>
       </c>
@@ -20362,7 +20422,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="399" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A399" s="1" t="s">
         <v>1024</v>
       </c>
@@ -20400,7 +20460,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="400" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A400" s="1" t="s">
         <v>1027</v>
       </c>
@@ -20438,7 +20498,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="401" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A401" s="1" t="s">
         <v>1030</v>
       </c>
@@ -20473,7 +20533,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="402" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A402" s="1" t="s">
         <v>1033</v>
       </c>
@@ -20508,7 +20568,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="403" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A403" s="1" t="s">
         <v>1036</v>
       </c>
@@ -20546,7 +20606,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="404" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A404" s="1" t="s">
         <v>1038</v>
       </c>
@@ -20581,7 +20641,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="405" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A405" s="1" t="s">
         <v>1041</v>
       </c>
@@ -20619,7 +20679,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="406" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A406" s="1" t="s">
         <v>1043</v>
       </c>
@@ -20657,7 +20717,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="407" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A407" s="1" t="s">
         <v>1046</v>
       </c>
@@ -20695,7 +20755,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="408" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A408" s="1" t="s">
         <v>1049</v>
       </c>
@@ -20730,7 +20790,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="409" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A409" s="1" t="s">
         <v>1052</v>
       </c>
@@ -20768,7 +20828,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="410" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A410" s="1" t="s">
         <v>1055</v>
       </c>
@@ -20806,7 +20866,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="411" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A411" s="1" t="s">
         <v>1058</v>
       </c>
@@ -20844,7 +20904,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="412" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A412" s="1" t="s">
         <v>1061</v>
       </c>
@@ -20882,7 +20942,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="413" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A413" s="1" t="s">
         <v>1064</v>
       </c>
@@ -20920,7 +20980,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="414" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A414" s="1" t="s">
         <v>1067</v>
       </c>
@@ -20958,7 +21018,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="415" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A415" s="1" t="s">
         <v>1070</v>
       </c>
@@ -20996,7 +21056,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="416" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A416" s="1" t="s">
         <v>1072</v>
       </c>
@@ -21034,7 +21094,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="417" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A417" s="1" t="s">
         <v>1075</v>
       </c>
@@ -21072,7 +21132,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="418" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A418" s="1" t="s">
         <v>1078</v>
       </c>
@@ -21110,7 +21170,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="419" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A419" s="1" t="s">
         <v>1089</v>
       </c>
@@ -21145,7 +21205,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="420" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A420" s="1" t="s">
         <v>1093</v>
       </c>
@@ -21180,7 +21240,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="421" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A421" s="1" t="s">
         <v>1096</v>
       </c>
@@ -21218,7 +21278,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="422" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A422" s="1" t="s">
         <v>1099</v>
       </c>
@@ -21253,7 +21313,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="423" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A423" s="1" t="s">
         <v>1101</v>
       </c>
@@ -21288,7 +21348,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="424" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A424" s="1" t="s">
         <v>1109</v>
       </c>
@@ -21323,7 +21383,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="425" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A425" s="1" t="s">
         <v>1113</v>
       </c>
@@ -21361,7 +21421,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="426" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A426" s="1" t="s">
         <v>1116</v>
       </c>
@@ -21396,7 +21456,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="427" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A427" s="1" t="s">
         <v>1118</v>
       </c>
@@ -21434,7 +21494,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="428" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A428" s="1" t="s">
         <v>1121</v>
       </c>
@@ -21472,7 +21532,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="429" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A429" s="1" t="s">
         <v>1124</v>
       </c>
@@ -21510,7 +21570,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="430" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A430" s="1" t="s">
         <v>1129</v>
       </c>
@@ -21548,7 +21608,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="431" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A431" s="1" t="s">
         <v>1086</v>
       </c>
@@ -21583,7 +21643,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="432" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A432" s="1" t="s">
         <v>1131</v>
       </c>
@@ -21621,7 +21681,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="433" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A433" s="1" t="s">
         <v>1134</v>
       </c>
@@ -21659,7 +21719,7 @@
         <v>1134</v>
       </c>
     </row>
-    <row r="434" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A434" s="1" t="s">
         <v>1137</v>
       </c>
@@ -21697,7 +21757,7 @@
         <v>1137</v>
       </c>
     </row>
-    <row r="435" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A435" s="1" t="s">
         <v>1140</v>
       </c>
@@ -21735,7 +21795,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="436" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A436" s="1" t="s">
         <v>1143</v>
       </c>
@@ -21773,7 +21833,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="437" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A437" s="1" t="s">
         <v>1145</v>
       </c>
@@ -21808,7 +21868,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="438" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A438" s="1" t="s">
         <v>1149</v>
       </c>
@@ -21846,7 +21906,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="439" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A439" s="1" t="s">
         <v>1152</v>
       </c>
@@ -21881,7 +21941,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="440" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A440" s="1" t="s">
         <v>1155</v>
       </c>
@@ -21919,7 +21979,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="441" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A441" s="1" t="s">
         <v>1157</v>
       </c>
@@ -21954,7 +22014,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="442" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A442" s="1" t="s">
         <v>1161</v>
       </c>
@@ -21989,7 +22049,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="443" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A443" s="1" t="s">
         <v>1164</v>
       </c>
@@ -22024,7 +22084,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="444" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A444" s="1" t="s">
         <v>1167</v>
       </c>
@@ -22059,7 +22119,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="445" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A445" s="1" t="s">
         <v>1171</v>
       </c>
@@ -22094,7 +22154,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="446" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A446" s="1" t="s">
         <v>1174</v>
       </c>
@@ -22129,7 +22189,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="447" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A447" s="1" t="s">
         <v>1179</v>
       </c>
@@ -22167,7 +22227,7 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="448" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A448" s="1" t="s">
         <v>1181</v>
       </c>
@@ -22205,7 +22265,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="449" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A449" s="1" t="s">
         <v>1187</v>
       </c>
@@ -22240,7 +22300,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="450" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A450" s="1" t="s">
         <v>1190</v>
       </c>
@@ -22275,7 +22335,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="451" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A451" s="1" t="s">
         <v>1193</v>
       </c>
@@ -22313,7 +22373,7 @@
         <v>1193</v>
       </c>
     </row>
-    <row r="452" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A452" s="1" t="s">
         <v>1196</v>
       </c>
@@ -22351,7 +22411,7 @@
         <v>1196</v>
       </c>
     </row>
-    <row r="453" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A453" s="1" t="s">
         <v>1199</v>
       </c>
@@ -22386,7 +22446,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="454" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A454" s="1" t="s">
         <v>1202</v>
       </c>
@@ -22424,7 +22484,7 @@
         <v>1202</v>
       </c>
     </row>
-    <row r="455" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A455" s="1" t="s">
         <v>1204</v>
       </c>
@@ -22462,7 +22522,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="456" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A456" s="1" t="s">
         <v>1206</v>
       </c>
@@ -22497,7 +22557,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="457" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A457" s="1" t="s">
         <v>1208</v>
       </c>
@@ -22535,7 +22595,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="458" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A458" s="1" t="s">
         <v>1211</v>
       </c>
@@ -22573,7 +22633,7 @@
         <v>1211</v>
       </c>
     </row>
-    <row r="459" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A459" s="1" t="s">
         <v>1214</v>
       </c>
@@ -22611,7 +22671,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="460" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A460" s="1" t="s">
         <v>1217</v>
       </c>
@@ -22646,7 +22706,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="461" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A461" s="1" t="s">
         <v>1219</v>
       </c>
@@ -22681,7 +22741,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="462" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A462" s="1" t="s">
         <v>1222</v>
       </c>
@@ -22716,7 +22776,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="463" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="N463">
         <f>COUNTIF(N2:N462,"*")</f>
         <v>263</v>
@@ -22745,8 +22805,12 @@
       <formula>ISBLANK($N2)</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="R309" r:id="rId1" display="https://www.haskell.org/platform/" xr:uid="{3B7247BA-B3CD-4AA3-9DBE-9EC23EBD2E0E}"/>
+    <hyperlink ref="P311" r:id="rId2" display="https://github.com/UCL-ARC/hpc-spack/issues/14" xr:uid="{C437DFB9-770E-408B-BC00-27DDF58D67AE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -22758,12 +22822,12 @@
       <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" s="4">
         <v>44903</v>
       </c>
@@ -22771,352 +22835,352 @@
         <v>1496</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>1497</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>1498</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>1499</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>1500</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>1501</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>1502</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>1503</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>1504</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>1505</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>1506</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>1507</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>1508</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>1509</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>1510</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>1511</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>1512</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>1513</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>1514</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>1515</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>1516</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>1517</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>1518</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>1519</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>1520</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>1521</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>1522</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>1523</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>1533</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>1534</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>1535</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>1536</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>1535</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>1537</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>1538</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>1535</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>1539</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>1540</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>1541</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>1535</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>1542</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
         <v>1543</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
         <v>1535</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
         <v>1544</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
         <v>1545</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
         <v>1535</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
         <v>1546</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
         <v>1535</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
         <v>1547</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
         <v>1548</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
         <v>1549</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
         <v>1551</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B66" t="s">
         <v>1552</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
         <v>1553</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
         <v>1554</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
         <v>1555</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
         <v>1556</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B71" t="s">
         <v>1557</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B72" t="s">
         <v>1558</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B73" t="s">
         <v>1559</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
         <v>1560</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B75" t="s">
         <v>1561</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B76" t="s">
         <v>1562</v>
       </c>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B77" t="s">
         <v>1563</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B78" t="s">
         <v>1564</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
         <v>1565</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B80" t="s">
         <v>1566</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
         <v>1567</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B83" t="s">
         <v>1568</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B84" t="s">
         <v>1569</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B85" t="s">
         <v>1570</v>
       </c>

</xml_diff>

<commit_message>
parsed_modules.xlsx - these notes updated to current env yaml files
</commit_message>
<xml_diff>
--- a/parsed_modules.xlsx
+++ b/parsed_modules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\james\hpc-spack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DFF209B-5870-4DA2-8977-C98645E18B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AF1DE0-6EDA-4DCE-8CF7-8A0FBF917C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-195" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parsed_modules" sheetId="1" r:id="rId1"/>
@@ -33,30 +33,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5467" uniqueCount="1599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5502" uniqueCount="1631">
   <si>
     <t>package</t>
   </si>
@@ -4849,10 +4827,106 @@
     <t>newer-there are lots of options</t>
   </si>
   <si>
-    <t>1.14.1</t>
-  </si>
-  <si>
     <t>OLDER but this is spack preferred</t>
+  </si>
+  <si>
+    <t>- latest - there are lots of options - mpi is an option</t>
+  </si>
+  <si>
+    <t>2.1-3</t>
+  </si>
+  <si>
+    <t>-only option and what we have</t>
+  </si>
+  <si>
+    <t>lastest - 9.3.2 id depreated by spack</t>
+  </si>
+  <si>
+    <t>3.4.0</t>
+  </si>
+  <si>
+    <t>a slight upgrade</t>
+  </si>
+  <si>
+    <t>0.188</t>
+  </si>
+  <si>
+    <t>many versions upgrade</t>
+  </si>
+  <si>
+    <t>there are options</t>
+  </si>
+  <si>
+    <t>3.3.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">latesst an don eof what we have </t>
+  </si>
+  <si>
+    <t>9.6.1</t>
+  </si>
+  <si>
+    <t>2017.113</t>
+  </si>
+  <si>
+    <t>many updates presumably</t>
+  </si>
+  <si>
+    <t>downgrade because 9.6.2 not in spack - there are options</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>20220205</t>
+  </si>
+  <si>
+    <t>one update</t>
+  </si>
+  <si>
+    <t>3.8.1</t>
+  </si>
+  <si>
+    <t>several updates - thre are options</t>
+  </si>
+  <si>
+    <t>2.5.2</t>
+  </si>
+  <si>
+    <t>a few updates</t>
+  </si>
+  <si>
+    <t>1.14.0</t>
+  </si>
+  <si>
+    <t>a few updates - there are options</t>
+  </si>
+  <si>
+    <t>1.14</t>
+  </si>
+  <si>
+    <t>2.20.0.422</t>
+  </si>
+  <si>
+    <t>an update?</t>
+  </si>
+  <si>
+    <t>1.3.0</t>
+  </si>
+  <si>
+    <t>2.4.2</t>
+  </si>
+  <si>
+    <t>0.7.17</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>latest and what we have - there are options</t>
   </si>
 </sst>
 </file>
@@ -5358,7 +5432,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -5371,6 +5445,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5761,9 +5839,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A346" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N362" sqref="N362"/>
+      <selection pane="topRight" activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5785,7 +5863,7 @@
     <col min="16" max="16" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5826,7 +5904,7 @@
         <v>1494</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>43</v>
       </c>
@@ -5861,7 +5939,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
@@ -5898,8 +5976,14 @@
       <c r="N3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O3" s="7" t="s">
+        <v>1609</v>
+      </c>
+      <c r="P3" t="s">
+        <v>1612</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>53</v>
       </c>
@@ -5936,8 +6020,14 @@
       <c r="N4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O4" s="5" t="s">
+        <v>1610</v>
+      </c>
+      <c r="P4" t="s">
+        <v>1611</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>56</v>
       </c>
@@ -5972,7 +6062,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>59</v>
       </c>
@@ -6009,8 +6099,11 @@
       <c r="N6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O6" s="8" t="s">
+        <v>1613</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>64</v>
       </c>
@@ -6045,7 +6138,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>67</v>
       </c>
@@ -6082,8 +6175,14 @@
       <c r="N8" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O8" s="5" t="s">
+        <v>1614</v>
+      </c>
+      <c r="P8" t="s">
+        <v>1615</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>70</v>
       </c>
@@ -6118,7 +6217,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>73</v>
       </c>
@@ -6155,8 +6254,14 @@
       <c r="N10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O10" t="s">
+        <v>1616</v>
+      </c>
+      <c r="P10" t="s">
+        <v>1617</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>76</v>
       </c>
@@ -6191,7 +6296,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>79</v>
       </c>
@@ -6226,7 +6331,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>82</v>
       </c>
@@ -6263,8 +6368,14 @@
       <c r="N13" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O13" t="s">
+        <v>1618</v>
+      </c>
+      <c r="P13" t="s">
+        <v>1619</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>85</v>
       </c>
@@ -6301,8 +6412,14 @@
       <c r="N14" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O14" s="5" t="s">
+        <v>1622</v>
+      </c>
+      <c r="P14" t="s">
+        <v>1621</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>88</v>
       </c>
@@ -6337,7 +6454,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>91</v>
       </c>
@@ -6374,8 +6491,14 @@
       <c r="N16" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O16" t="s">
+        <v>1623</v>
+      </c>
+      <c r="P16" t="s">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>94</v>
       </c>
@@ -6410,7 +6533,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>97</v>
       </c>
@@ -6445,7 +6568,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>100</v>
       </c>
@@ -6480,7 +6603,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>103</v>
       </c>
@@ -6515,7 +6638,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>106</v>
       </c>
@@ -6550,7 +6673,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>109</v>
       </c>
@@ -6585,7 +6708,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>112</v>
       </c>
@@ -6620,7 +6743,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>116</v>
       </c>
@@ -6657,8 +6780,14 @@
       <c r="N24" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O24" t="s">
+        <v>1625</v>
+      </c>
+      <c r="P24" t="s">
+        <v>1621</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>119</v>
       </c>
@@ -6695,8 +6824,14 @@
       <c r="N25" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O25" t="s">
+        <v>1626</v>
+      </c>
+      <c r="P25" t="s">
+        <v>1619</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>122</v>
       </c>
@@ -6733,13 +6868,19 @@
       <c r="N26" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O26" t="s">
+        <v>1627</v>
+      </c>
+      <c r="P26" t="s">
+        <v>1619</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>16</v>
+      <c r="B27" s="9" t="s">
+        <v>1628</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>12</v>
@@ -6771,8 +6912,14 @@
       <c r="N27" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O27" s="5" t="s">
+        <v>1629</v>
+      </c>
+      <c r="P27" t="s">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>136</v>
       </c>
@@ -6807,7 +6954,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>140</v>
       </c>
@@ -6845,7 +6992,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>143</v>
       </c>
@@ -6883,7 +7030,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>147</v>
       </c>
@@ -6918,7 +7065,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>150</v>
       </c>
@@ -18822,7 +18969,7 @@
         <v>1588</v>
       </c>
     </row>
-    <row r="353" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A353" s="1" t="s">
         <v>876</v>
       </c>
@@ -18866,7 +19013,7 @@
         <v>1590</v>
       </c>
     </row>
-    <row r="354" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
         <v>882</v>
       </c>
@@ -18907,7 +19054,7 @@
         <v>1591</v>
       </c>
     </row>
-    <row r="355" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
         <v>885</v>
       </c>
@@ -18942,7 +19089,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="356" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
         <v>888</v>
       </c>
@@ -18982,12 +19129,11 @@
       <c r="O356" s="7" t="s">
         <v>1592</v>
       </c>
-      <c r="P356" t="e" cm="1">
-        <f t="array" ref="P356">- latest - there are lots of options - mpi is an option</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="357" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P356" s="5" t="s">
+        <v>1598</v>
+      </c>
+    </row>
+    <row r="357" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A357" s="1" t="s">
         <v>894</v>
       </c>
@@ -19022,7 +19168,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="358" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
         <v>897</v>
       </c>
@@ -19066,7 +19212,7 @@
         <v>1594</v>
       </c>
     </row>
-    <row r="359" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A359" s="1" t="s">
         <v>900</v>
       </c>
@@ -19110,7 +19256,7 @@
         <v>1596</v>
       </c>
     </row>
-    <row r="360" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
         <v>903</v>
       </c>
@@ -19145,7 +19291,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="361" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A361" s="1" t="s">
         <v>906</v>
       </c>
@@ -19183,13 +19329,13 @@
         <v>906</v>
       </c>
       <c r="O361" t="s">
+        <v>1620</v>
+      </c>
+      <c r="P361" t="s">
         <v>1597</v>
       </c>
-      <c r="P361" t="s">
-        <v>1598</v>
-      </c>
-    </row>
-    <row r="362" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="362" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
         <v>909</v>
       </c>
@@ -19226,8 +19372,14 @@
       <c r="N362" t="s">
         <v>909</v>
       </c>
-    </row>
-    <row r="363" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O362" t="s">
+        <v>1599</v>
+      </c>
+      <c r="P362" s="5" t="s">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="363" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A363" s="1" t="s">
         <v>912</v>
       </c>
@@ -19262,7 +19414,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="364" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
         <v>914</v>
       </c>
@@ -19299,8 +19451,14 @@
       <c r="N364" t="s">
         <v>914</v>
       </c>
-    </row>
-    <row r="365" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O364" t="s">
+        <v>1528</v>
+      </c>
+      <c r="P364" t="s">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="365" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A365" s="1" t="s">
         <v>917</v>
       </c>
@@ -19337,8 +19495,14 @@
       <c r="N365" t="s">
         <v>917</v>
       </c>
-    </row>
-    <row r="366" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O365" t="s">
+        <v>1602</v>
+      </c>
+      <c r="P365" t="s">
+        <v>1603</v>
+      </c>
+    </row>
+    <row r="366" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A366" s="1" t="s">
         <v>920</v>
       </c>
@@ -19375,8 +19539,17 @@
       <c r="N366" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="367" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O366" s="5" t="s">
+        <v>1604</v>
+      </c>
+      <c r="P366" t="s">
+        <v>1605</v>
+      </c>
+      <c r="Q366" t="s">
+        <v>1606</v>
+      </c>
+    </row>
+    <row r="367" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A367" s="1" t="s">
         <v>923</v>
       </c>
@@ -19413,8 +19586,14 @@
       <c r="N367" t="s">
         <v>923</v>
       </c>
-    </row>
-    <row r="368" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O367" s="7" t="s">
+        <v>1607</v>
+      </c>
+      <c r="P367" t="s">
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="368" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A368" s="1" t="s">
         <v>930</v>
       </c>
@@ -22932,7 +23111,7 @@
       <formula>"NONE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N462 O286 O288:P288 O313:P313 O210:P210 P351:P352 O349:O354 O356 O358:P359 O361:P361">
+  <conditionalFormatting sqref="N2:N462 O286 O288:P288 O313:P313 O210:P210 P351:P352 O349:O354 O356 O358:P359 O361:P361 O362 Q366 O364:P367 O3:P3 P4 O8:P8 O10:P10 O13:P13 O24:P26 P27">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>$L2</formula>
     </cfRule>

</xml_diff>